<commit_message>
update các màn hình điều phối, nhập, xuất và xuất theo bộ
</commit_message>
<xml_diff>
--- a/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/Cap nhat phieu nhap kho/WF0011 Cap nhat phieu nhap kho.xlsx
+++ b/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/Cap nhat phieu nhap kho/WF0011 Cap nhat phieu nhap kho.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" tabRatio="791" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Update History" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="6">'Form Func Spec'!$A$1:$K$54</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="7">'Func Spec'!$A$1:$K$29</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="8">Help!$A$1:$Q$63</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">'Input Check'!$A$1:$L$14</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'Input Check'!$A$1:$L$13</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'Item Screen'!$A$1:$N$34</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Layout Screen'!$A$1:$J$8</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Update History'!$A$1:$J$14</definedName>
@@ -1147,30 +1147,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ngày tạo tài liệu</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -1952,7 +1928,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="321">
   <si>
     <t>Detail Design</t>
   </si>
@@ -3397,11 +3373,6 @@
     <t>@SQL011</t>
   </si>
   <si>
-    <t>SELECT TOP 1 1 FROM AT2006
-WHERE DivisionID = @DivisionID
-AND VoucherID = @VoucherID AND IsWeb=1</t>
-  </si>
-  <si>
     <t>@DivisionID @VoucherID  
 @IsWeb</t>
   </si>
@@ -3414,36 +3385,65 @@
     <t>Ver 6.0</t>
   </si>
   <si>
-    <t>Sửa</t>
-  </si>
-  <si>
-    <t>Require</t>
-  </si>
-  <si>
-    <t>Click</t>
-  </si>
-  <si>
-    <t>WFML000186</t>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>CustomizeIndex</t>
   </si>
   <si>
     <t>-CustomizeIndex = 51 (Hoàng Trần) 
-+ Sheet Input Check thêm WFML000186
 + Sheet Data Input Thêm @SQL009
 + Sheet Form Func Spec thêm xử lý khi sửa</t>
   </si>
   <si>
-    <t>Chỉ dùng Customize Hoàng Trần (CustomizeIndex = 51) Kiểm tra điều kiện nhập Web khi thực hiện sửa Phiếu nhập</t>
-  </si>
-  <si>
-    <t>CustomizeIndex = 51: Click LinkEdit  thực thi câu @SQL009 kiểm tra điều kiện IsWeb 
-+ Nếu =1 Warn message WFML000186, Click Ok thực hiện @SQL004 load Form WF0011 Chỉ Enabled trường Description , RefNo01, RefNo02, ActualQuantity, Ana01ID, Ana02ID, Ana03ID, Ana04ID, Ana05ID, Ana06ID, Ana07ID, Ana08ID, Ana09ID, Ana10ID, PeriodID, ProductID để sửa còn lại Disabled. Click No thoát ra 
+    <r>
+      <t xml:space="preserve">SELECT TOP 1 1 FROM AT2006
+WHERE DivisionID = @DivisionID
+AND VoucherID = @VoucherID AND </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>IsWeb=1</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kiểm tra điều kiện nhập Web khi thực hiện sửa Phiếu nhập</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>Luồng nghiệp vụ 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="0"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+CustomizeIndex = 51: Click LinkEdit  thực thi câu @SQL011 kiểm tra điều kiện IsWeb 
++ Nếu =1 Warn message WFML000186, Click Yes thực hiện @SQL004 load Form WF0011 Chỉ Enabled trường Description , RefNo01, RefNo02, ActualQuantity, Ana01ID, Ana02ID, Ana03ID, Ana04ID, Ana05ID, Ana06ID, Ana07ID, Ana08ID, Ana09ID, Ana10ID, PeriodID, ProductID để sửa còn lại Disabled. Click No thoát ra 
 + Nếu =0 thực thi @SQL004 load giá trị cho Form WF0011</t>
-  </si>
-  <si>
-    <t>Version</t>
-  </si>
-  <si>
-    <t>CustomizeIndex</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Ver 6.0  </t>
+  </si>
+  <si>
+    <t>Tham khảo luồng nghiệp vụ 1</t>
   </si>
 </sst>
 </file>
@@ -3453,7 +3453,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3583,6 +3583,13 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color theme="0"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="9"/>
       <color theme="0"/>
       <name val="Tahoma"/>
@@ -3912,7 +3919,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="373">
+  <cellXfs count="366">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4670,18 +4677,6 @@
     <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4851,15 +4846,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5565,7 +5551,7 @@
   <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10:J10"/>
+      <selection activeCell="E11" sqref="E11:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5584,10 +5570,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="284" t="s">
+      <c r="A1" s="280" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="284"/>
+      <c r="B1" s="280"/>
       <c r="C1" s="46" t="s">
         <v>1</v>
       </c>
@@ -5614,8 +5600,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="284"/>
-      <c r="B2" s="284"/>
+      <c r="A2" s="280"/>
+      <c r="B2" s="280"/>
       <c r="C2" s="46" t="s">
         <v>7</v>
       </c>
@@ -5666,14 +5652,14 @@
       <c r="D4" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="285" t="s">
+      <c r="E4" s="281" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="285"/>
-      <c r="G4" s="285"/>
-      <c r="H4" s="285"/>
-      <c r="I4" s="285"/>
-      <c r="J4" s="285"/>
+      <c r="F4" s="281"/>
+      <c r="G4" s="281"/>
+      <c r="H4" s="281"/>
+      <c r="I4" s="281"/>
+      <c r="J4" s="281"/>
     </row>
     <row r="5" spans="1:10" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18">
@@ -5690,14 +5676,14 @@
         <f>H1</f>
         <v>Thanh Sơn</v>
       </c>
-      <c r="E5" s="286" t="s">
+      <c r="E5" s="282" t="s">
         <v>172</v>
       </c>
-      <c r="F5" s="287"/>
-      <c r="G5" s="287"/>
-      <c r="H5" s="287"/>
-      <c r="I5" s="287"/>
-      <c r="J5" s="287"/>
+      <c r="F5" s="283"/>
+      <c r="G5" s="283"/>
+      <c r="H5" s="283"/>
+      <c r="I5" s="283"/>
+      <c r="J5" s="283"/>
     </row>
     <row r="6" spans="1:10" s="111" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
@@ -5712,14 +5698,14 @@
       <c r="D6" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="288" t="s">
+      <c r="E6" s="284" t="s">
         <v>240</v>
       </c>
-      <c r="F6" s="289"/>
-      <c r="G6" s="289"/>
-      <c r="H6" s="289"/>
-      <c r="I6" s="289"/>
-      <c r="J6" s="290"/>
+      <c r="F6" s="285"/>
+      <c r="G6" s="285"/>
+      <c r="H6" s="285"/>
+      <c r="I6" s="285"/>
+      <c r="J6" s="286"/>
     </row>
     <row r="7" spans="1:10" s="30" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="187">
@@ -5734,14 +5720,14 @@
       <c r="D7" s="190" t="s">
         <v>250</v>
       </c>
-      <c r="E7" s="291" t="s">
+      <c r="E7" s="287" t="s">
         <v>251</v>
       </c>
-      <c r="F7" s="292"/>
-      <c r="G7" s="292"/>
-      <c r="H7" s="292"/>
-      <c r="I7" s="292"/>
-      <c r="J7" s="293"/>
+      <c r="F7" s="288"/>
+      <c r="G7" s="288"/>
+      <c r="H7" s="288"/>
+      <c r="I7" s="288"/>
+      <c r="J7" s="289"/>
     </row>
     <row r="8" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -5756,14 +5742,14 @@
       <c r="D8" s="23" t="s">
         <v>250</v>
       </c>
-      <c r="E8" s="281" t="s">
+      <c r="E8" s="277" t="s">
         <v>279</v>
       </c>
-      <c r="F8" s="282"/>
-      <c r="G8" s="282"/>
-      <c r="H8" s="282"/>
-      <c r="I8" s="282"/>
-      <c r="J8" s="283"/>
+      <c r="F8" s="278"/>
+      <c r="G8" s="278"/>
+      <c r="H8" s="278"/>
+      <c r="I8" s="278"/>
+      <c r="J8" s="279"/>
     </row>
     <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -5778,14 +5764,14 @@
       <c r="D9" s="26" t="s">
         <v>250</v>
       </c>
-      <c r="E9" s="295" t="s">
+      <c r="E9" s="291" t="s">
         <v>300</v>
       </c>
-      <c r="F9" s="296"/>
-      <c r="G9" s="296"/>
-      <c r="H9" s="296"/>
-      <c r="I9" s="296"/>
-      <c r="J9" s="297"/>
+      <c r="F9" s="292"/>
+      <c r="G9" s="292"/>
+      <c r="H9" s="292"/>
+      <c r="I9" s="292"/>
+      <c r="J9" s="293"/>
     </row>
     <row r="10" spans="1:10" s="30" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -5800,14 +5786,14 @@
       <c r="D10" s="114" t="s">
         <v>304</v>
       </c>
-      <c r="E10" s="298" t="s">
-        <v>318</v>
-      </c>
-      <c r="F10" s="299"/>
-      <c r="G10" s="299"/>
-      <c r="H10" s="299"/>
-      <c r="I10" s="299"/>
-      <c r="J10" s="300"/>
+      <c r="E10" s="294" t="s">
+        <v>315</v>
+      </c>
+      <c r="F10" s="295"/>
+      <c r="G10" s="295"/>
+      <c r="H10" s="295"/>
+      <c r="I10" s="295"/>
+      <c r="J10" s="296"/>
     </row>
     <row r="11" spans="1:10" s="30" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
@@ -5818,12 +5804,12 @@
       </c>
       <c r="C11" s="116"/>
       <c r="D11" s="117"/>
-      <c r="E11" s="301"/>
-      <c r="F11" s="302"/>
-      <c r="G11" s="302"/>
-      <c r="H11" s="302"/>
-      <c r="I11" s="302"/>
-      <c r="J11" s="303"/>
+      <c r="E11" s="297"/>
+      <c r="F11" s="298"/>
+      <c r="G11" s="298"/>
+      <c r="H11" s="298"/>
+      <c r="I11" s="298"/>
+      <c r="J11" s="299"/>
     </row>
     <row r="12" spans="1:10" s="30" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
@@ -5834,12 +5820,12 @@
       </c>
       <c r="C12" s="119"/>
       <c r="D12" s="120"/>
-      <c r="E12" s="304"/>
-      <c r="F12" s="305"/>
-      <c r="G12" s="305"/>
-      <c r="H12" s="305"/>
-      <c r="I12" s="305"/>
-      <c r="J12" s="306"/>
+      <c r="E12" s="300"/>
+      <c r="F12" s="301"/>
+      <c r="G12" s="301"/>
+      <c r="H12" s="301"/>
+      <c r="I12" s="301"/>
+      <c r="J12" s="302"/>
     </row>
     <row r="13" spans="1:10" s="30" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
@@ -5850,12 +5836,12 @@
       </c>
       <c r="C13" s="28"/>
       <c r="D13" s="29"/>
-      <c r="E13" s="307"/>
-      <c r="F13" s="308"/>
-      <c r="G13" s="308"/>
-      <c r="H13" s="308"/>
-      <c r="I13" s="308"/>
-      <c r="J13" s="309"/>
+      <c r="E13" s="303"/>
+      <c r="F13" s="304"/>
+      <c r="G13" s="304"/>
+      <c r="H13" s="304"/>
+      <c r="I13" s="304"/>
+      <c r="J13" s="305"/>
     </row>
     <row r="14" spans="1:10" s="30" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
@@ -5866,348 +5852,348 @@
       </c>
       <c r="C14" s="32"/>
       <c r="D14" s="33"/>
-      <c r="E14" s="310"/>
-      <c r="F14" s="311"/>
-      <c r="G14" s="311"/>
-      <c r="H14" s="311"/>
-      <c r="I14" s="311"/>
-      <c r="J14" s="312"/>
+      <c r="E14" s="306"/>
+      <c r="F14" s="307"/>
+      <c r="G14" s="307"/>
+      <c r="H14" s="307"/>
+      <c r="I14" s="307"/>
+      <c r="J14" s="308"/>
     </row>
     <row r="15" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A15" s="34"/>
       <c r="B15" s="35"/>
       <c r="C15" s="36"/>
       <c r="D15" s="34"/>
-      <c r="E15" s="294"/>
-      <c r="F15" s="294"/>
-      <c r="G15" s="294"/>
-      <c r="H15" s="294"/>
-      <c r="I15" s="294"/>
-      <c r="J15" s="294"/>
+      <c r="E15" s="290"/>
+      <c r="F15" s="290"/>
+      <c r="G15" s="290"/>
+      <c r="H15" s="290"/>
+      <c r="I15" s="290"/>
+      <c r="J15" s="290"/>
     </row>
     <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="35"/>
       <c r="C16" s="36"/>
       <c r="D16" s="34"/>
-      <c r="E16" s="294"/>
-      <c r="F16" s="294"/>
-      <c r="G16" s="294"/>
-      <c r="H16" s="294"/>
-      <c r="I16" s="294"/>
-      <c r="J16" s="294"/>
+      <c r="E16" s="290"/>
+      <c r="F16" s="290"/>
+      <c r="G16" s="290"/>
+      <c r="H16" s="290"/>
+      <c r="I16" s="290"/>
+      <c r="J16" s="290"/>
     </row>
     <row r="17" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="35"/>
       <c r="C17" s="36"/>
       <c r="D17" s="34"/>
-      <c r="E17" s="294"/>
-      <c r="F17" s="294"/>
-      <c r="G17" s="294"/>
-      <c r="H17" s="294"/>
-      <c r="I17" s="294"/>
-      <c r="J17" s="294"/>
+      <c r="E17" s="290"/>
+      <c r="F17" s="290"/>
+      <c r="G17" s="290"/>
+      <c r="H17" s="290"/>
+      <c r="I17" s="290"/>
+      <c r="J17" s="290"/>
     </row>
     <row r="18" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="35"/>
       <c r="C18" s="36"/>
       <c r="D18" s="34"/>
-      <c r="E18" s="294"/>
-      <c r="F18" s="294"/>
-      <c r="G18" s="294"/>
-      <c r="H18" s="294"/>
-      <c r="I18" s="294"/>
-      <c r="J18" s="294"/>
+      <c r="E18" s="290"/>
+      <c r="F18" s="290"/>
+      <c r="G18" s="290"/>
+      <c r="H18" s="290"/>
+      <c r="I18" s="290"/>
+      <c r="J18" s="290"/>
     </row>
     <row r="19" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="35"/>
       <c r="C19" s="36"/>
       <c r="D19" s="34"/>
-      <c r="E19" s="294"/>
-      <c r="F19" s="294"/>
-      <c r="G19" s="294"/>
-      <c r="H19" s="294"/>
-      <c r="I19" s="294"/>
-      <c r="J19" s="294"/>
+      <c r="E19" s="290"/>
+      <c r="F19" s="290"/>
+      <c r="G19" s="290"/>
+      <c r="H19" s="290"/>
+      <c r="I19" s="290"/>
+      <c r="J19" s="290"/>
     </row>
     <row r="20" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="35"/>
       <c r="C20" s="36"/>
       <c r="D20" s="34"/>
-      <c r="E20" s="294"/>
-      <c r="F20" s="294"/>
-      <c r="G20" s="294"/>
-      <c r="H20" s="294"/>
-      <c r="I20" s="294"/>
-      <c r="J20" s="294"/>
+      <c r="E20" s="290"/>
+      <c r="F20" s="290"/>
+      <c r="G20" s="290"/>
+      <c r="H20" s="290"/>
+      <c r="I20" s="290"/>
+      <c r="J20" s="290"/>
     </row>
     <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="35"/>
       <c r="C21" s="36"/>
       <c r="D21" s="34"/>
-      <c r="E21" s="294"/>
-      <c r="F21" s="294"/>
-      <c r="G21" s="294"/>
-      <c r="H21" s="294"/>
-      <c r="I21" s="294"/>
-      <c r="J21" s="294"/>
+      <c r="E21" s="290"/>
+      <c r="F21" s="290"/>
+      <c r="G21" s="290"/>
+      <c r="H21" s="290"/>
+      <c r="I21" s="290"/>
+      <c r="J21" s="290"/>
     </row>
     <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="35"/>
       <c r="C22" s="36"/>
       <c r="D22" s="34"/>
-      <c r="E22" s="294"/>
-      <c r="F22" s="294"/>
-      <c r="G22" s="294"/>
-      <c r="H22" s="294"/>
-      <c r="I22" s="294"/>
-      <c r="J22" s="294"/>
+      <c r="E22" s="290"/>
+      <c r="F22" s="290"/>
+      <c r="G22" s="290"/>
+      <c r="H22" s="290"/>
+      <c r="I22" s="290"/>
+      <c r="J22" s="290"/>
     </row>
     <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="35"/>
       <c r="C23" s="36"/>
       <c r="D23" s="34"/>
-      <c r="E23" s="294"/>
-      <c r="F23" s="294"/>
-      <c r="G23" s="294"/>
-      <c r="H23" s="294"/>
-      <c r="I23" s="294"/>
-      <c r="J23" s="294"/>
+      <c r="E23" s="290"/>
+      <c r="F23" s="290"/>
+      <c r="G23" s="290"/>
+      <c r="H23" s="290"/>
+      <c r="I23" s="290"/>
+      <c r="J23" s="290"/>
     </row>
     <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="35"/>
       <c r="C24" s="36"/>
       <c r="D24" s="34"/>
-      <c r="E24" s="294"/>
-      <c r="F24" s="294"/>
-      <c r="G24" s="294"/>
-      <c r="H24" s="294"/>
-      <c r="I24" s="294"/>
-      <c r="J24" s="294"/>
+      <c r="E24" s="290"/>
+      <c r="F24" s="290"/>
+      <c r="G24" s="290"/>
+      <c r="H24" s="290"/>
+      <c r="I24" s="290"/>
+      <c r="J24" s="290"/>
     </row>
     <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A25" s="34"/>
       <c r="B25" s="35"/>
       <c r="C25" s="36"/>
       <c r="D25" s="34"/>
-      <c r="E25" s="294"/>
-      <c r="F25" s="294"/>
-      <c r="G25" s="294"/>
-      <c r="H25" s="294"/>
-      <c r="I25" s="294"/>
-      <c r="J25" s="294"/>
+      <c r="E25" s="290"/>
+      <c r="F25" s="290"/>
+      <c r="G25" s="290"/>
+      <c r="H25" s="290"/>
+      <c r="I25" s="290"/>
+      <c r="J25" s="290"/>
     </row>
     <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="35"/>
       <c r="C26" s="36"/>
       <c r="D26" s="34"/>
-      <c r="E26" s="294"/>
-      <c r="F26" s="294"/>
-      <c r="G26" s="294"/>
-      <c r="H26" s="294"/>
-      <c r="I26" s="294"/>
-      <c r="J26" s="294"/>
+      <c r="E26" s="290"/>
+      <c r="F26" s="290"/>
+      <c r="G26" s="290"/>
+      <c r="H26" s="290"/>
+      <c r="I26" s="290"/>
+      <c r="J26" s="290"/>
     </row>
     <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="35"/>
       <c r="C27" s="36"/>
       <c r="D27" s="34"/>
-      <c r="E27" s="294"/>
-      <c r="F27" s="294"/>
-      <c r="G27" s="294"/>
-      <c r="H27" s="294"/>
-      <c r="I27" s="294"/>
-      <c r="J27" s="294"/>
+      <c r="E27" s="290"/>
+      <c r="F27" s="290"/>
+      <c r="G27" s="290"/>
+      <c r="H27" s="290"/>
+      <c r="I27" s="290"/>
+      <c r="J27" s="290"/>
     </row>
     <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="35"/>
       <c r="C28" s="36"/>
       <c r="D28" s="34"/>
-      <c r="E28" s="294"/>
-      <c r="F28" s="294"/>
-      <c r="G28" s="294"/>
-      <c r="H28" s="294"/>
-      <c r="I28" s="294"/>
-      <c r="J28" s="294"/>
+      <c r="E28" s="290"/>
+      <c r="F28" s="290"/>
+      <c r="G28" s="290"/>
+      <c r="H28" s="290"/>
+      <c r="I28" s="290"/>
+      <c r="J28" s="290"/>
     </row>
     <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="35"/>
       <c r="C29" s="36"/>
       <c r="D29" s="34"/>
-      <c r="E29" s="294"/>
-      <c r="F29" s="294"/>
-      <c r="G29" s="294"/>
-      <c r="H29" s="294"/>
-      <c r="I29" s="294"/>
-      <c r="J29" s="294"/>
+      <c r="E29" s="290"/>
+      <c r="F29" s="290"/>
+      <c r="G29" s="290"/>
+      <c r="H29" s="290"/>
+      <c r="I29" s="290"/>
+      <c r="J29" s="290"/>
     </row>
     <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="35"/>
       <c r="C30" s="36"/>
       <c r="D30" s="34"/>
-      <c r="E30" s="294"/>
-      <c r="F30" s="294"/>
-      <c r="G30" s="294"/>
-      <c r="H30" s="294"/>
-      <c r="I30" s="294"/>
-      <c r="J30" s="294"/>
+      <c r="E30" s="290"/>
+      <c r="F30" s="290"/>
+      <c r="G30" s="290"/>
+      <c r="H30" s="290"/>
+      <c r="I30" s="290"/>
+      <c r="J30" s="290"/>
     </row>
     <row r="31" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="35"/>
       <c r="C31" s="36"/>
       <c r="D31" s="34"/>
-      <c r="E31" s="294"/>
-      <c r="F31" s="294"/>
-      <c r="G31" s="294"/>
-      <c r="H31" s="294"/>
-      <c r="I31" s="294"/>
-      <c r="J31" s="294"/>
+      <c r="E31" s="290"/>
+      <c r="F31" s="290"/>
+      <c r="G31" s="290"/>
+      <c r="H31" s="290"/>
+      <c r="I31" s="290"/>
+      <c r="J31" s="290"/>
     </row>
     <row r="32" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="35"/>
       <c r="C32" s="36"/>
       <c r="D32" s="34"/>
-      <c r="E32" s="294"/>
-      <c r="F32" s="294"/>
-      <c r="G32" s="294"/>
-      <c r="H32" s="294"/>
-      <c r="I32" s="294"/>
-      <c r="J32" s="294"/>
+      <c r="E32" s="290"/>
+      <c r="F32" s="290"/>
+      <c r="G32" s="290"/>
+      <c r="H32" s="290"/>
+      <c r="I32" s="290"/>
+      <c r="J32" s="290"/>
     </row>
     <row r="33" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="35"/>
       <c r="C33" s="36"/>
       <c r="D33" s="34"/>
-      <c r="E33" s="294"/>
-      <c r="F33" s="294"/>
-      <c r="G33" s="294"/>
-      <c r="H33" s="294"/>
-      <c r="I33" s="294"/>
-      <c r="J33" s="294"/>
+      <c r="E33" s="290"/>
+      <c r="F33" s="290"/>
+      <c r="G33" s="290"/>
+      <c r="H33" s="290"/>
+      <c r="I33" s="290"/>
+      <c r="J33" s="290"/>
     </row>
     <row r="34" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="35"/>
       <c r="C34" s="36"/>
       <c r="D34" s="34"/>
-      <c r="E34" s="294"/>
-      <c r="F34" s="294"/>
-      <c r="G34" s="294"/>
-      <c r="H34" s="294"/>
-      <c r="I34" s="294"/>
-      <c r="J34" s="294"/>
+      <c r="E34" s="290"/>
+      <c r="F34" s="290"/>
+      <c r="G34" s="290"/>
+      <c r="H34" s="290"/>
+      <c r="I34" s="290"/>
+      <c r="J34" s="290"/>
     </row>
     <row r="35" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A35" s="34"/>
       <c r="B35" s="35"/>
       <c r="C35" s="36"/>
       <c r="D35" s="34"/>
-      <c r="E35" s="294"/>
-      <c r="F35" s="294"/>
-      <c r="G35" s="294"/>
-      <c r="H35" s="294"/>
-      <c r="I35" s="294"/>
-      <c r="J35" s="294"/>
+      <c r="E35" s="290"/>
+      <c r="F35" s="290"/>
+      <c r="G35" s="290"/>
+      <c r="H35" s="290"/>
+      <c r="I35" s="290"/>
+      <c r="J35" s="290"/>
     </row>
     <row r="36" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="35"/>
       <c r="C36" s="36"/>
       <c r="D36" s="34"/>
-      <c r="E36" s="294"/>
-      <c r="F36" s="294"/>
-      <c r="G36" s="294"/>
-      <c r="H36" s="294"/>
-      <c r="I36" s="294"/>
-      <c r="J36" s="294"/>
+      <c r="E36" s="290"/>
+      <c r="F36" s="290"/>
+      <c r="G36" s="290"/>
+      <c r="H36" s="290"/>
+      <c r="I36" s="290"/>
+      <c r="J36" s="290"/>
     </row>
     <row r="37" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="35"/>
       <c r="C37" s="36"/>
       <c r="D37" s="34"/>
-      <c r="E37" s="294"/>
-      <c r="F37" s="294"/>
-      <c r="G37" s="294"/>
-      <c r="H37" s="294"/>
-      <c r="I37" s="294"/>
-      <c r="J37" s="294"/>
+      <c r="E37" s="290"/>
+      <c r="F37" s="290"/>
+      <c r="G37" s="290"/>
+      <c r="H37" s="290"/>
+      <c r="I37" s="290"/>
+      <c r="J37" s="290"/>
     </row>
     <row r="38" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="35"/>
       <c r="C38" s="36"/>
       <c r="D38" s="34"/>
-      <c r="E38" s="294"/>
-      <c r="F38" s="294"/>
-      <c r="G38" s="294"/>
-      <c r="H38" s="294"/>
-      <c r="I38" s="294"/>
-      <c r="J38" s="294"/>
+      <c r="E38" s="290"/>
+      <c r="F38" s="290"/>
+      <c r="G38" s="290"/>
+      <c r="H38" s="290"/>
+      <c r="I38" s="290"/>
+      <c r="J38" s="290"/>
     </row>
     <row r="39" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="35"/>
       <c r="C39" s="36"/>
       <c r="D39" s="34"/>
-      <c r="E39" s="294"/>
-      <c r="F39" s="294"/>
-      <c r="G39" s="294"/>
-      <c r="H39" s="294"/>
-      <c r="I39" s="294"/>
-      <c r="J39" s="294"/>
+      <c r="E39" s="290"/>
+      <c r="F39" s="290"/>
+      <c r="G39" s="290"/>
+      <c r="H39" s="290"/>
+      <c r="I39" s="290"/>
+      <c r="J39" s="290"/>
     </row>
     <row r="40" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="35"/>
       <c r="C40" s="36"/>
       <c r="D40" s="34"/>
-      <c r="E40" s="294"/>
-      <c r="F40" s="294"/>
-      <c r="G40" s="294"/>
-      <c r="H40" s="294"/>
-      <c r="I40" s="294"/>
-      <c r="J40" s="294"/>
+      <c r="E40" s="290"/>
+      <c r="F40" s="290"/>
+      <c r="G40" s="290"/>
+      <c r="H40" s="290"/>
+      <c r="I40" s="290"/>
+      <c r="J40" s="290"/>
     </row>
     <row r="41" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="35"/>
       <c r="C41" s="36"/>
       <c r="D41" s="34"/>
-      <c r="E41" s="294"/>
-      <c r="F41" s="294"/>
-      <c r="G41" s="294"/>
-      <c r="H41" s="294"/>
-      <c r="I41" s="294"/>
-      <c r="J41" s="294"/>
+      <c r="E41" s="290"/>
+      <c r="F41" s="290"/>
+      <c r="G41" s="290"/>
+      <c r="H41" s="290"/>
+      <c r="I41" s="290"/>
+      <c r="J41" s="290"/>
     </row>
     <row r="42" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="35"/>
       <c r="C42" s="36"/>
       <c r="D42" s="34"/>
-      <c r="E42" s="294"/>
-      <c r="F42" s="294"/>
-      <c r="G42" s="294"/>
-      <c r="H42" s="294"/>
-      <c r="I42" s="294"/>
-      <c r="J42" s="294"/>
+      <c r="E42" s="290"/>
+      <c r="F42" s="290"/>
+      <c r="G42" s="290"/>
+      <c r="H42" s="290"/>
+      <c r="I42" s="290"/>
+      <c r="J42" s="290"/>
     </row>
   </sheetData>
   <mergeCells count="40">
@@ -6459,10 +6445,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="284" t="s">
+      <c r="A1" s="280" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="284"/>
+      <c r="B1" s="280"/>
       <c r="C1" s="46" t="s">
         <v>1</v>
       </c>
@@ -6493,8 +6479,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="284"/>
-      <c r="B2" s="284"/>
+      <c r="A2" s="280"/>
+      <c r="B2" s="280"/>
       <c r="C2" s="46" t="s">
         <v>7</v>
       </c>
@@ -6537,76 +6523,76 @@
       <c r="J3" s="17"/>
     </row>
     <row r="4" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="284" t="s">
+      <c r="A4" s="280" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="284"/>
-      <c r="C4" s="284"/>
-      <c r="D4" s="284"/>
-      <c r="E4" s="284"/>
-      <c r="F4" s="284"/>
-      <c r="G4" s="284"/>
-      <c r="H4" s="284"/>
-      <c r="I4" s="284" t="s">
+      <c r="B4" s="280"/>
+      <c r="C4" s="280"/>
+      <c r="D4" s="280"/>
+      <c r="E4" s="280"/>
+      <c r="F4" s="280"/>
+      <c r="G4" s="280"/>
+      <c r="H4" s="280"/>
+      <c r="I4" s="280" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="284"/>
+      <c r="J4" s="280"/>
     </row>
     <row r="5" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="321"/>
-      <c r="B5" s="322"/>
-      <c r="C5" s="322"/>
-      <c r="D5" s="322"/>
-      <c r="E5" s="322"/>
-      <c r="F5" s="322"/>
-      <c r="G5" s="322"/>
-      <c r="H5" s="323"/>
-      <c r="I5" s="313" t="s">
+      <c r="A5" s="317"/>
+      <c r="B5" s="318"/>
+      <c r="C5" s="318"/>
+      <c r="D5" s="318"/>
+      <c r="E5" s="318"/>
+      <c r="F5" s="318"/>
+      <c r="G5" s="318"/>
+      <c r="H5" s="319"/>
+      <c r="I5" s="309" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="314"/>
+      <c r="J5" s="310"/>
     </row>
     <row r="6" spans="1:10" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="324"/>
-      <c r="B6" s="325"/>
-      <c r="C6" s="325"/>
-      <c r="D6" s="325"/>
-      <c r="E6" s="325"/>
-      <c r="F6" s="325"/>
-      <c r="G6" s="325"/>
-      <c r="H6" s="326"/>
-      <c r="I6" s="315" t="s">
+      <c r="A6" s="320"/>
+      <c r="B6" s="321"/>
+      <c r="C6" s="321"/>
+      <c r="D6" s="321"/>
+      <c r="E6" s="321"/>
+      <c r="F6" s="321"/>
+      <c r="G6" s="321"/>
+      <c r="H6" s="322"/>
+      <c r="I6" s="311" t="s">
         <v>247</v>
       </c>
-      <c r="J6" s="316"/>
+      <c r="J6" s="312"/>
     </row>
     <row r="7" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="324"/>
-      <c r="B7" s="325"/>
-      <c r="C7" s="325"/>
-      <c r="D7" s="325"/>
-      <c r="E7" s="325"/>
-      <c r="F7" s="325"/>
-      <c r="G7" s="325"/>
-      <c r="H7" s="326"/>
-      <c r="I7" s="317" t="s">
+      <c r="A7" s="320"/>
+      <c r="B7" s="321"/>
+      <c r="C7" s="321"/>
+      <c r="D7" s="321"/>
+      <c r="E7" s="321"/>
+      <c r="F7" s="321"/>
+      <c r="G7" s="321"/>
+      <c r="H7" s="322"/>
+      <c r="I7" s="313" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="318"/>
+      <c r="J7" s="314"/>
     </row>
     <row r="8" spans="1:10" ht="336" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="324"/>
-      <c r="B8" s="325"/>
-      <c r="C8" s="325"/>
-      <c r="D8" s="325"/>
-      <c r="E8" s="325"/>
-      <c r="F8" s="325"/>
-      <c r="G8" s="325"/>
-      <c r="H8" s="326"/>
-      <c r="I8" s="319" t="s">
+      <c r="A8" s="320"/>
+      <c r="B8" s="321"/>
+      <c r="C8" s="321"/>
+      <c r="D8" s="321"/>
+      <c r="E8" s="321"/>
+      <c r="F8" s="321"/>
+      <c r="G8" s="321"/>
+      <c r="H8" s="322"/>
+      <c r="I8" s="315" t="s">
         <v>241</v>
       </c>
-      <c r="J8" s="320"/>
+      <c r="J8" s="316"/>
     </row>
     <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
@@ -6685,336 +6671,336 @@
       <c r="B15" s="35"/>
       <c r="C15" s="36"/>
       <c r="D15" s="34"/>
-      <c r="E15" s="294"/>
-      <c r="F15" s="294"/>
-      <c r="G15" s="294"/>
-      <c r="H15" s="294"/>
-      <c r="I15" s="294"/>
-      <c r="J15" s="294"/>
+      <c r="E15" s="290"/>
+      <c r="F15" s="290"/>
+      <c r="G15" s="290"/>
+      <c r="H15" s="290"/>
+      <c r="I15" s="290"/>
+      <c r="J15" s="290"/>
     </row>
     <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="35"/>
       <c r="C16" s="36"/>
       <c r="D16" s="34"/>
-      <c r="E16" s="294"/>
-      <c r="F16" s="294"/>
-      <c r="G16" s="294"/>
-      <c r="H16" s="294"/>
-      <c r="I16" s="294"/>
-      <c r="J16" s="294"/>
+      <c r="E16" s="290"/>
+      <c r="F16" s="290"/>
+      <c r="G16" s="290"/>
+      <c r="H16" s="290"/>
+      <c r="I16" s="290"/>
+      <c r="J16" s="290"/>
     </row>
     <row r="17" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="35"/>
       <c r="C17" s="36"/>
       <c r="D17" s="34"/>
-      <c r="E17" s="294"/>
-      <c r="F17" s="294"/>
-      <c r="G17" s="294"/>
-      <c r="H17" s="294"/>
-      <c r="I17" s="294"/>
-      <c r="J17" s="294"/>
+      <c r="E17" s="290"/>
+      <c r="F17" s="290"/>
+      <c r="G17" s="290"/>
+      <c r="H17" s="290"/>
+      <c r="I17" s="290"/>
+      <c r="J17" s="290"/>
     </row>
     <row r="18" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="35"/>
       <c r="C18" s="36"/>
       <c r="D18" s="34"/>
-      <c r="E18" s="294"/>
-      <c r="F18" s="294"/>
-      <c r="G18" s="294"/>
-      <c r="H18" s="294"/>
-      <c r="I18" s="294"/>
-      <c r="J18" s="294"/>
+      <c r="E18" s="290"/>
+      <c r="F18" s="290"/>
+      <c r="G18" s="290"/>
+      <c r="H18" s="290"/>
+      <c r="I18" s="290"/>
+      <c r="J18" s="290"/>
     </row>
     <row r="19" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="35"/>
       <c r="C19" s="36"/>
       <c r="D19" s="34"/>
-      <c r="E19" s="294"/>
-      <c r="F19" s="294"/>
-      <c r="G19" s="294"/>
-      <c r="H19" s="294"/>
-      <c r="I19" s="294"/>
-      <c r="J19" s="294"/>
+      <c r="E19" s="290"/>
+      <c r="F19" s="290"/>
+      <c r="G19" s="290"/>
+      <c r="H19" s="290"/>
+      <c r="I19" s="290"/>
+      <c r="J19" s="290"/>
     </row>
     <row r="20" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="35"/>
       <c r="C20" s="36"/>
       <c r="D20" s="34"/>
-      <c r="E20" s="294"/>
-      <c r="F20" s="294"/>
-      <c r="G20" s="294"/>
-      <c r="H20" s="294"/>
-      <c r="I20" s="294"/>
-      <c r="J20" s="294"/>
+      <c r="E20" s="290"/>
+      <c r="F20" s="290"/>
+      <c r="G20" s="290"/>
+      <c r="H20" s="290"/>
+      <c r="I20" s="290"/>
+      <c r="J20" s="290"/>
     </row>
     <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="35"/>
       <c r="C21" s="36"/>
       <c r="D21" s="34"/>
-      <c r="E21" s="294"/>
-      <c r="F21" s="294"/>
-      <c r="G21" s="294"/>
-      <c r="H21" s="294"/>
-      <c r="I21" s="294"/>
-      <c r="J21" s="294"/>
+      <c r="E21" s="290"/>
+      <c r="F21" s="290"/>
+      <c r="G21" s="290"/>
+      <c r="H21" s="290"/>
+      <c r="I21" s="290"/>
+      <c r="J21" s="290"/>
     </row>
     <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="35"/>
       <c r="C22" s="36"/>
       <c r="D22" s="34"/>
-      <c r="E22" s="294"/>
-      <c r="F22" s="294"/>
-      <c r="G22" s="294"/>
-      <c r="H22" s="294"/>
-      <c r="I22" s="294"/>
-      <c r="J22" s="294"/>
+      <c r="E22" s="290"/>
+      <c r="F22" s="290"/>
+      <c r="G22" s="290"/>
+      <c r="H22" s="290"/>
+      <c r="I22" s="290"/>
+      <c r="J22" s="290"/>
     </row>
     <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="35"/>
       <c r="C23" s="36"/>
       <c r="D23" s="34"/>
-      <c r="E23" s="294"/>
-      <c r="F23" s="294"/>
-      <c r="G23" s="294"/>
-      <c r="H23" s="294"/>
-      <c r="I23" s="294"/>
-      <c r="J23" s="294"/>
+      <c r="E23" s="290"/>
+      <c r="F23" s="290"/>
+      <c r="G23" s="290"/>
+      <c r="H23" s="290"/>
+      <c r="I23" s="290"/>
+      <c r="J23" s="290"/>
     </row>
     <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="35"/>
       <c r="C24" s="36"/>
       <c r="D24" s="34"/>
-      <c r="E24" s="294"/>
-      <c r="F24" s="294"/>
-      <c r="G24" s="294"/>
-      <c r="H24" s="294"/>
-      <c r="I24" s="294"/>
-      <c r="J24" s="294"/>
+      <c r="E24" s="290"/>
+      <c r="F24" s="290"/>
+      <c r="G24" s="290"/>
+      <c r="H24" s="290"/>
+      <c r="I24" s="290"/>
+      <c r="J24" s="290"/>
     </row>
     <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A25" s="34"/>
       <c r="B25" s="35"/>
       <c r="C25" s="36"/>
       <c r="D25" s="34"/>
-      <c r="E25" s="294"/>
-      <c r="F25" s="294"/>
-      <c r="G25" s="294"/>
-      <c r="H25" s="294"/>
-      <c r="I25" s="294"/>
-      <c r="J25" s="294"/>
+      <c r="E25" s="290"/>
+      <c r="F25" s="290"/>
+      <c r="G25" s="290"/>
+      <c r="H25" s="290"/>
+      <c r="I25" s="290"/>
+      <c r="J25" s="290"/>
     </row>
     <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="35"/>
       <c r="C26" s="36"/>
       <c r="D26" s="34"/>
-      <c r="E26" s="294"/>
-      <c r="F26" s="294"/>
-      <c r="G26" s="294"/>
-      <c r="H26" s="294"/>
-      <c r="I26" s="294"/>
-      <c r="J26" s="294"/>
+      <c r="E26" s="290"/>
+      <c r="F26" s="290"/>
+      <c r="G26" s="290"/>
+      <c r="H26" s="290"/>
+      <c r="I26" s="290"/>
+      <c r="J26" s="290"/>
     </row>
     <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="35"/>
       <c r="C27" s="36"/>
       <c r="D27" s="34"/>
-      <c r="E27" s="294"/>
-      <c r="F27" s="294"/>
-      <c r="G27" s="294"/>
-      <c r="H27" s="294"/>
-      <c r="I27" s="294"/>
-      <c r="J27" s="294"/>
+      <c r="E27" s="290"/>
+      <c r="F27" s="290"/>
+      <c r="G27" s="290"/>
+      <c r="H27" s="290"/>
+      <c r="I27" s="290"/>
+      <c r="J27" s="290"/>
     </row>
     <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="35"/>
       <c r="C28" s="36"/>
       <c r="D28" s="34"/>
-      <c r="E28" s="294"/>
-      <c r="F28" s="294"/>
-      <c r="G28" s="294"/>
-      <c r="H28" s="294"/>
-      <c r="I28" s="294"/>
-      <c r="J28" s="294"/>
+      <c r="E28" s="290"/>
+      <c r="F28" s="290"/>
+      <c r="G28" s="290"/>
+      <c r="H28" s="290"/>
+      <c r="I28" s="290"/>
+      <c r="J28" s="290"/>
     </row>
     <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="35"/>
       <c r="C29" s="36"/>
       <c r="D29" s="34"/>
-      <c r="E29" s="294"/>
-      <c r="F29" s="294"/>
-      <c r="G29" s="294"/>
-      <c r="H29" s="294"/>
-      <c r="I29" s="294"/>
-      <c r="J29" s="294"/>
+      <c r="E29" s="290"/>
+      <c r="F29" s="290"/>
+      <c r="G29" s="290"/>
+      <c r="H29" s="290"/>
+      <c r="I29" s="290"/>
+      <c r="J29" s="290"/>
     </row>
     <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="35"/>
       <c r="C30" s="36"/>
       <c r="D30" s="34"/>
-      <c r="E30" s="294"/>
-      <c r="F30" s="294"/>
-      <c r="G30" s="294"/>
-      <c r="H30" s="294"/>
-      <c r="I30" s="294"/>
-      <c r="J30" s="294"/>
+      <c r="E30" s="290"/>
+      <c r="F30" s="290"/>
+      <c r="G30" s="290"/>
+      <c r="H30" s="290"/>
+      <c r="I30" s="290"/>
+      <c r="J30" s="290"/>
     </row>
     <row r="31" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="35"/>
       <c r="C31" s="36"/>
       <c r="D31" s="34"/>
-      <c r="E31" s="294"/>
-      <c r="F31" s="294"/>
-      <c r="G31" s="294"/>
-      <c r="H31" s="294"/>
-      <c r="I31" s="294"/>
-      <c r="J31" s="294"/>
+      <c r="E31" s="290"/>
+      <c r="F31" s="290"/>
+      <c r="G31" s="290"/>
+      <c r="H31" s="290"/>
+      <c r="I31" s="290"/>
+      <c r="J31" s="290"/>
     </row>
     <row r="32" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="35"/>
       <c r="C32" s="36"/>
       <c r="D32" s="34"/>
-      <c r="E32" s="294"/>
-      <c r="F32" s="294"/>
-      <c r="G32" s="294"/>
-      <c r="H32" s="294"/>
-      <c r="I32" s="294"/>
-      <c r="J32" s="294"/>
+      <c r="E32" s="290"/>
+      <c r="F32" s="290"/>
+      <c r="G32" s="290"/>
+      <c r="H32" s="290"/>
+      <c r="I32" s="290"/>
+      <c r="J32" s="290"/>
     </row>
     <row r="33" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="35"/>
       <c r="C33" s="36"/>
       <c r="D33" s="34"/>
-      <c r="E33" s="294"/>
-      <c r="F33" s="294"/>
-      <c r="G33" s="294"/>
-      <c r="H33" s="294"/>
-      <c r="I33" s="294"/>
-      <c r="J33" s="294"/>
+      <c r="E33" s="290"/>
+      <c r="F33" s="290"/>
+      <c r="G33" s="290"/>
+      <c r="H33" s="290"/>
+      <c r="I33" s="290"/>
+      <c r="J33" s="290"/>
     </row>
     <row r="34" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="35"/>
       <c r="C34" s="36"/>
       <c r="D34" s="34"/>
-      <c r="E34" s="294"/>
-      <c r="F34" s="294"/>
-      <c r="G34" s="294"/>
-      <c r="H34" s="294"/>
-      <c r="I34" s="294"/>
-      <c r="J34" s="294"/>
+      <c r="E34" s="290"/>
+      <c r="F34" s="290"/>
+      <c r="G34" s="290"/>
+      <c r="H34" s="290"/>
+      <c r="I34" s="290"/>
+      <c r="J34" s="290"/>
     </row>
     <row r="35" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A35" s="34"/>
       <c r="B35" s="35"/>
       <c r="C35" s="36"/>
       <c r="D35" s="34"/>
-      <c r="E35" s="294"/>
-      <c r="F35" s="294"/>
-      <c r="G35" s="294"/>
-      <c r="H35" s="294"/>
-      <c r="I35" s="294"/>
-      <c r="J35" s="294"/>
+      <c r="E35" s="290"/>
+      <c r="F35" s="290"/>
+      <c r="G35" s="290"/>
+      <c r="H35" s="290"/>
+      <c r="I35" s="290"/>
+      <c r="J35" s="290"/>
     </row>
     <row r="36" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="35"/>
       <c r="C36" s="36"/>
       <c r="D36" s="34"/>
-      <c r="E36" s="294"/>
-      <c r="F36" s="294"/>
-      <c r="G36" s="294"/>
-      <c r="H36" s="294"/>
-      <c r="I36" s="294"/>
-      <c r="J36" s="294"/>
+      <c r="E36" s="290"/>
+      <c r="F36" s="290"/>
+      <c r="G36" s="290"/>
+      <c r="H36" s="290"/>
+      <c r="I36" s="290"/>
+      <c r="J36" s="290"/>
     </row>
     <row r="37" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="35"/>
       <c r="C37" s="36"/>
       <c r="D37" s="34"/>
-      <c r="E37" s="294"/>
-      <c r="F37" s="294"/>
-      <c r="G37" s="294"/>
-      <c r="H37" s="294"/>
-      <c r="I37" s="294"/>
-      <c r="J37" s="294"/>
+      <c r="E37" s="290"/>
+      <c r="F37" s="290"/>
+      <c r="G37" s="290"/>
+      <c r="H37" s="290"/>
+      <c r="I37" s="290"/>
+      <c r="J37" s="290"/>
     </row>
     <row r="38" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="35"/>
       <c r="C38" s="36"/>
       <c r="D38" s="34"/>
-      <c r="E38" s="294"/>
-      <c r="F38" s="294"/>
-      <c r="G38" s="294"/>
-      <c r="H38" s="294"/>
-      <c r="I38" s="294"/>
-      <c r="J38" s="294"/>
+      <c r="E38" s="290"/>
+      <c r="F38" s="290"/>
+      <c r="G38" s="290"/>
+      <c r="H38" s="290"/>
+      <c r="I38" s="290"/>
+      <c r="J38" s="290"/>
     </row>
     <row r="39" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="35"/>
       <c r="C39" s="36"/>
       <c r="D39" s="34"/>
-      <c r="E39" s="294"/>
-      <c r="F39" s="294"/>
-      <c r="G39" s="294"/>
-      <c r="H39" s="294"/>
-      <c r="I39" s="294"/>
-      <c r="J39" s="294"/>
+      <c r="E39" s="290"/>
+      <c r="F39" s="290"/>
+      <c r="G39" s="290"/>
+      <c r="H39" s="290"/>
+      <c r="I39" s="290"/>
+      <c r="J39" s="290"/>
     </row>
     <row r="40" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="35"/>
       <c r="C40" s="36"/>
       <c r="D40" s="34"/>
-      <c r="E40" s="294"/>
-      <c r="F40" s="294"/>
-      <c r="G40" s="294"/>
-      <c r="H40" s="294"/>
-      <c r="I40" s="294"/>
-      <c r="J40" s="294"/>
+      <c r="E40" s="290"/>
+      <c r="F40" s="290"/>
+      <c r="G40" s="290"/>
+      <c r="H40" s="290"/>
+      <c r="I40" s="290"/>
+      <c r="J40" s="290"/>
     </row>
     <row r="41" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="35"/>
       <c r="C41" s="36"/>
       <c r="D41" s="34"/>
-      <c r="E41" s="294"/>
-      <c r="F41" s="294"/>
-      <c r="G41" s="294"/>
-      <c r="H41" s="294"/>
-      <c r="I41" s="294"/>
-      <c r="J41" s="294"/>
+      <c r="E41" s="290"/>
+      <c r="F41" s="290"/>
+      <c r="G41" s="290"/>
+      <c r="H41" s="290"/>
+      <c r="I41" s="290"/>
+      <c r="J41" s="290"/>
     </row>
     <row r="42" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="35"/>
       <c r="C42" s="36"/>
       <c r="D42" s="34"/>
-      <c r="E42" s="294"/>
-      <c r="F42" s="294"/>
-      <c r="G42" s="294"/>
-      <c r="H42" s="294"/>
-      <c r="I42" s="294"/>
-      <c r="J42" s="294"/>
+      <c r="E42" s="290"/>
+      <c r="F42" s="290"/>
+      <c r="G42" s="290"/>
+      <c r="H42" s="290"/>
+      <c r="I42" s="290"/>
+      <c r="J42" s="290"/>
     </row>
   </sheetData>
   <mergeCells count="36">
@@ -7095,10 +7081,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="284" t="s">
+      <c r="A1" s="280" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="327"/>
+      <c r="B1" s="323"/>
       <c r="C1" s="124" t="s">
         <v>1</v>
       </c>
@@ -7123,18 +7109,18 @@
       <c r="I1" s="124" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="328" t="str">
+      <c r="J1" s="324" t="str">
         <f>'Update History'!J1</f>
         <v>Thị Phượng</v>
       </c>
-      <c r="K1" s="329"/>
+      <c r="K1" s="325"/>
       <c r="L1" s="17"/>
       <c r="M1" s="17"/>
       <c r="N1" s="17"/>
     </row>
     <row r="2" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="284"/>
-      <c r="B2" s="327"/>
+      <c r="A2" s="280"/>
+      <c r="B2" s="323"/>
       <c r="C2" s="124" t="s">
         <v>7</v>
       </c>
@@ -7159,11 +7145,11 @@
       <c r="I2" s="124" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="330">
+      <c r="J2" s="326">
         <f>'Update History'!J2</f>
         <v>42381</v>
       </c>
-      <c r="K2" s="331"/>
+      <c r="K2" s="327"/>
       <c r="L2" s="17"/>
       <c r="M2" s="17"/>
       <c r="N2" s="17"/>
@@ -8873,10 +8859,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L42"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8894,12 +8880,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="284" t="s">
+      <c r="A1" s="280" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="284"/>
-      <c r="C1" s="284"/>
-      <c r="D1" s="284"/>
+      <c r="B1" s="280"/>
+      <c r="C1" s="280"/>
+      <c r="D1" s="280"/>
       <c r="E1" s="46" t="s">
         <v>1</v>
       </c>
@@ -8930,10 +8916,10 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="284"/>
-      <c r="B2" s="284"/>
-      <c r="C2" s="284"/>
-      <c r="D2" s="284"/>
+      <c r="A2" s="280"/>
+      <c r="B2" s="280"/>
+      <c r="C2" s="280"/>
+      <c r="D2" s="280"/>
       <c r="E2" s="46" t="s">
         <v>7</v>
       </c>
@@ -8981,11 +8967,11 @@
       <c r="A4" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="279" t="s">
-        <v>321</v>
-      </c>
-      <c r="C4" s="279" t="s">
-        <v>322</v>
+      <c r="B4" s="275" t="s">
+        <v>313</v>
+      </c>
+      <c r="C4" s="275" t="s">
+        <v>314</v>
       </c>
       <c r="D4" s="61" t="s">
         <v>22</v>
@@ -9005,67 +8991,53 @@
       <c r="I4" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="335" t="s">
+      <c r="J4" s="331" t="s">
         <v>37</v>
       </c>
-      <c r="K4" s="335"/>
-      <c r="L4" s="335"/>
-    </row>
-    <row r="5" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="114"/>
-      <c r="B5" s="114" t="s">
-        <v>313</v>
-      </c>
-      <c r="C5" s="114">
-        <v>51</v>
-      </c>
-      <c r="D5" s="112" t="s">
-        <v>314</v>
-      </c>
-      <c r="E5" s="275" t="s">
-        <v>315</v>
-      </c>
-      <c r="F5" s="276"/>
-      <c r="G5" s="277"/>
-      <c r="H5" s="278" t="s">
-        <v>307</v>
-      </c>
-      <c r="I5" s="278" t="s">
-        <v>316</v>
-      </c>
-      <c r="J5" s="336" t="s">
-        <v>317</v>
-      </c>
-      <c r="K5" s="337"/>
-      <c r="L5" s="338"/>
+      <c r="K4" s="331"/>
+      <c r="L4" s="331"/>
+    </row>
+    <row r="5" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="52"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="55"/>
+      <c r="J5" s="328"/>
+      <c r="K5" s="329"/>
+      <c r="L5" s="330"/>
     </row>
     <row r="6" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="52"/>
-      <c r="B6" s="52"/>
-      <c r="C6" s="52"/>
+      <c r="A6" s="56"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
       <c r="D6" s="19"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="332"/>
-      <c r="K6" s="333"/>
-      <c r="L6" s="334"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="328"/>
+      <c r="K6" s="329"/>
+      <c r="L6" s="330"/>
     </row>
     <row r="7" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="56"/>
-      <c r="B7" s="56"/>
-      <c r="C7" s="56"/>
+      <c r="A7" s="52"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="52"/>
       <c r="D7" s="19"/>
       <c r="E7" s="57"/>
       <c r="F7" s="18"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="332"/>
-      <c r="K7" s="333"/>
-      <c r="L7" s="334"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="328"/>
+      <c r="K7" s="329"/>
+      <c r="L7" s="330"/>
     </row>
     <row r="8" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="52"/>
@@ -9074,26 +9046,26 @@
       <c r="D8" s="19"/>
       <c r="E8" s="57"/>
       <c r="F8" s="18"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="50"/>
-      <c r="I8" s="50"/>
-      <c r="J8" s="332"/>
-      <c r="K8" s="333"/>
-      <c r="L8" s="334"/>
+      <c r="G8" s="51"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="328"/>
+      <c r="K8" s="329"/>
+      <c r="L8" s="330"/>
     </row>
     <row r="9" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="52"/>
-      <c r="B9" s="52"/>
-      <c r="C9" s="52"/>
+      <c r="A9" s="56"/>
+      <c r="B9" s="56"/>
+      <c r="C9" s="56"/>
       <c r="D9" s="19"/>
       <c r="E9" s="57"/>
       <c r="F9" s="18"/>
       <c r="G9" s="51"/>
       <c r="H9" s="51"/>
       <c r="I9" s="51"/>
-      <c r="J9" s="332"/>
-      <c r="K9" s="333"/>
-      <c r="L9" s="334"/>
+      <c r="J9" s="328"/>
+      <c r="K9" s="329"/>
+      <c r="L9" s="330"/>
     </row>
     <row r="10" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="56"/>
@@ -9105,9 +9077,9 @@
       <c r="G10" s="51"/>
       <c r="H10" s="51"/>
       <c r="I10" s="51"/>
-      <c r="J10" s="332"/>
-      <c r="K10" s="333"/>
-      <c r="L10" s="334"/>
+      <c r="J10" s="328"/>
+      <c r="K10" s="329"/>
+      <c r="L10" s="330"/>
     </row>
     <row r="11" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="56"/>
@@ -9119,23 +9091,23 @@
       <c r="G11" s="51"/>
       <c r="H11" s="51"/>
       <c r="I11" s="51"/>
-      <c r="J11" s="332"/>
-      <c r="K11" s="333"/>
-      <c r="L11" s="334"/>
-    </row>
-    <row r="12" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J11" s="328"/>
+      <c r="K11" s="329"/>
+      <c r="L11" s="330"/>
+    </row>
+    <row r="12" spans="1:12" s="30" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="56"/>
       <c r="B12" s="56"/>
       <c r="C12" s="56"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="51"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="51"/>
-      <c r="J12" s="332"/>
-      <c r="K12" s="333"/>
-      <c r="L12" s="334"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="55"/>
+      <c r="H12" s="55"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="328"/>
+      <c r="K12" s="329"/>
+      <c r="L12" s="330"/>
     </row>
     <row r="13" spans="1:12" s="30" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="56"/>
@@ -9147,65 +9119,65 @@
       <c r="G13" s="55"/>
       <c r="H13" s="55"/>
       <c r="I13" s="55"/>
-      <c r="J13" s="332"/>
-      <c r="K13" s="333"/>
-      <c r="L13" s="334"/>
-    </row>
-    <row r="14" spans="1:12" s="30" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="56"/>
-      <c r="B14" s="56"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="55"/>
-      <c r="H14" s="55"/>
-      <c r="I14" s="55"/>
-      <c r="J14" s="332"/>
-      <c r="K14" s="333"/>
-      <c r="L14" s="334"/>
+      <c r="J13" s="328"/>
+      <c r="K13" s="329"/>
+      <c r="L13" s="330"/>
+    </row>
+    <row r="14" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="34"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="290"/>
+      <c r="H14" s="290"/>
+      <c r="I14" s="290"/>
+      <c r="J14" s="290"/>
+      <c r="K14" s="290"/>
+      <c r="L14" s="290"/>
     </row>
     <row r="15" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="34"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
       <c r="D15" s="35"/>
       <c r="E15" s="36"/>
       <c r="F15" s="34"/>
-      <c r="G15" s="294"/>
-      <c r="H15" s="294"/>
-      <c r="I15" s="294"/>
-      <c r="J15" s="294"/>
-      <c r="K15" s="294"/>
-      <c r="L15" s="294"/>
+      <c r="G15" s="290"/>
+      <c r="H15" s="290"/>
+      <c r="I15" s="290"/>
+      <c r="J15" s="290"/>
+      <c r="K15" s="290"/>
+      <c r="L15" s="290"/>
     </row>
     <row r="16" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
       <c r="D16" s="35"/>
       <c r="E16" s="36"/>
       <c r="F16" s="34"/>
-      <c r="G16" s="294"/>
-      <c r="H16" s="294"/>
-      <c r="I16" s="294"/>
-      <c r="J16" s="294"/>
-      <c r="K16" s="294"/>
-      <c r="L16" s="294"/>
+      <c r="G16" s="290"/>
+      <c r="H16" s="290"/>
+      <c r="I16" s="290"/>
+      <c r="J16" s="290"/>
+      <c r="K16" s="290"/>
+      <c r="L16" s="290"/>
     </row>
     <row r="17" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
       <c r="D17" s="35"/>
       <c r="E17" s="36"/>
       <c r="F17" s="34"/>
-      <c r="G17" s="294"/>
-      <c r="H17" s="294"/>
-      <c r="I17" s="294"/>
-      <c r="J17" s="294"/>
-      <c r="K17" s="294"/>
-      <c r="L17" s="294"/>
+      <c r="G17" s="290"/>
+      <c r="H17" s="290"/>
+      <c r="I17" s="290"/>
+      <c r="J17" s="290"/>
+      <c r="K17" s="290"/>
+      <c r="L17" s="290"/>
     </row>
     <row r="18" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
@@ -9214,26 +9186,26 @@
       <c r="D18" s="35"/>
       <c r="E18" s="36"/>
       <c r="F18" s="34"/>
-      <c r="G18" s="294"/>
-      <c r="H18" s="294"/>
-      <c r="I18" s="294"/>
-      <c r="J18" s="294"/>
-      <c r="K18" s="294"/>
-      <c r="L18" s="294"/>
+      <c r="G18" s="290"/>
+      <c r="H18" s="290"/>
+      <c r="I18" s="290"/>
+      <c r="J18" s="290"/>
+      <c r="K18" s="290"/>
+      <c r="L18" s="290"/>
     </row>
     <row r="19" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
       <c r="D19" s="35"/>
       <c r="E19" s="36"/>
       <c r="F19" s="34"/>
-      <c r="G19" s="294"/>
-      <c r="H19" s="294"/>
-      <c r="I19" s="294"/>
-      <c r="J19" s="294"/>
-      <c r="K19" s="294"/>
-      <c r="L19" s="294"/>
+      <c r="G19" s="290"/>
+      <c r="H19" s="290"/>
+      <c r="I19" s="290"/>
+      <c r="J19" s="290"/>
+      <c r="K19" s="290"/>
+      <c r="L19" s="290"/>
     </row>
     <row r="20" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
@@ -9242,12 +9214,12 @@
       <c r="D20" s="35"/>
       <c r="E20" s="36"/>
       <c r="F20" s="34"/>
-      <c r="G20" s="294"/>
-      <c r="H20" s="294"/>
-      <c r="I20" s="294"/>
-      <c r="J20" s="294"/>
-      <c r="K20" s="294"/>
-      <c r="L20" s="294"/>
+      <c r="G20" s="290"/>
+      <c r="H20" s="290"/>
+      <c r="I20" s="290"/>
+      <c r="J20" s="290"/>
+      <c r="K20" s="290"/>
+      <c r="L20" s="290"/>
     </row>
     <row r="21" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
@@ -9256,12 +9228,12 @@
       <c r="D21" s="35"/>
       <c r="E21" s="36"/>
       <c r="F21" s="34"/>
-      <c r="G21" s="294"/>
-      <c r="H21" s="294"/>
-      <c r="I21" s="294"/>
-      <c r="J21" s="294"/>
-      <c r="K21" s="294"/>
-      <c r="L21" s="294"/>
+      <c r="G21" s="290"/>
+      <c r="H21" s="290"/>
+      <c r="I21" s="290"/>
+      <c r="J21" s="290"/>
+      <c r="K21" s="290"/>
+      <c r="L21" s="290"/>
     </row>
     <row r="22" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
@@ -9270,12 +9242,12 @@
       <c r="D22" s="35"/>
       <c r="E22" s="36"/>
       <c r="F22" s="34"/>
-      <c r="G22" s="294"/>
-      <c r="H22" s="294"/>
-      <c r="I22" s="294"/>
-      <c r="J22" s="294"/>
-      <c r="K22" s="294"/>
-      <c r="L22" s="294"/>
+      <c r="G22" s="290"/>
+      <c r="H22" s="290"/>
+      <c r="I22" s="290"/>
+      <c r="J22" s="290"/>
+      <c r="K22" s="290"/>
+      <c r="L22" s="290"/>
     </row>
     <row r="23" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
@@ -9284,68 +9256,68 @@
       <c r="D23" s="35"/>
       <c r="E23" s="36"/>
       <c r="F23" s="34"/>
-      <c r="G23" s="294"/>
-      <c r="H23" s="294"/>
-      <c r="I23" s="294"/>
-      <c r="J23" s="294"/>
-      <c r="K23" s="294"/>
-      <c r="L23" s="294"/>
+      <c r="G23" s="290"/>
+      <c r="H23" s="290"/>
+      <c r="I23" s="290"/>
+      <c r="J23" s="290"/>
+      <c r="K23" s="290"/>
+      <c r="L23" s="290"/>
     </row>
     <row r="24" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
+      <c r="A24" s="34"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="34"/>
       <c r="D24" s="35"/>
       <c r="E24" s="36"/>
       <c r="F24" s="34"/>
-      <c r="G24" s="294"/>
-      <c r="H24" s="294"/>
-      <c r="I24" s="294"/>
-      <c r="J24" s="294"/>
-      <c r="K24" s="294"/>
-      <c r="L24" s="294"/>
+      <c r="G24" s="290"/>
+      <c r="H24" s="290"/>
+      <c r="I24" s="290"/>
+      <c r="J24" s="290"/>
+      <c r="K24" s="290"/>
+      <c r="L24" s="290"/>
     </row>
     <row r="25" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="34"/>
-      <c r="B25" s="34"/>
-      <c r="C25" s="34"/>
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
       <c r="D25" s="35"/>
       <c r="E25" s="36"/>
       <c r="F25" s="34"/>
-      <c r="G25" s="294"/>
-      <c r="H25" s="294"/>
-      <c r="I25" s="294"/>
-      <c r="J25" s="294"/>
-      <c r="K25" s="294"/>
-      <c r="L25" s="294"/>
+      <c r="G25" s="290"/>
+      <c r="H25" s="290"/>
+      <c r="I25" s="290"/>
+      <c r="J25" s="290"/>
+      <c r="K25" s="290"/>
+      <c r="L25" s="290"/>
     </row>
     <row r="26" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
       <c r="D26" s="35"/>
       <c r="E26" s="36"/>
       <c r="F26" s="34"/>
-      <c r="G26" s="294"/>
-      <c r="H26" s="294"/>
-      <c r="I26" s="294"/>
-      <c r="J26" s="294"/>
-      <c r="K26" s="294"/>
-      <c r="L26" s="294"/>
+      <c r="G26" s="290"/>
+      <c r="H26" s="290"/>
+      <c r="I26" s="290"/>
+      <c r="J26" s="290"/>
+      <c r="K26" s="290"/>
+      <c r="L26" s="290"/>
     </row>
     <row r="27" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
       <c r="D27" s="35"/>
       <c r="E27" s="36"/>
       <c r="F27" s="34"/>
-      <c r="G27" s="294"/>
-      <c r="H27" s="294"/>
-      <c r="I27" s="294"/>
-      <c r="J27" s="294"/>
-      <c r="K27" s="294"/>
-      <c r="L27" s="294"/>
+      <c r="G27" s="290"/>
+      <c r="H27" s="290"/>
+      <c r="I27" s="290"/>
+      <c r="J27" s="290"/>
+      <c r="K27" s="290"/>
+      <c r="L27" s="290"/>
     </row>
     <row r="28" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
@@ -9354,26 +9326,26 @@
       <c r="D28" s="35"/>
       <c r="E28" s="36"/>
       <c r="F28" s="34"/>
-      <c r="G28" s="294"/>
-      <c r="H28" s="294"/>
-      <c r="I28" s="294"/>
-      <c r="J28" s="294"/>
-      <c r="K28" s="294"/>
-      <c r="L28" s="294"/>
+      <c r="G28" s="290"/>
+      <c r="H28" s="290"/>
+      <c r="I28" s="290"/>
+      <c r="J28" s="290"/>
+      <c r="K28" s="290"/>
+      <c r="L28" s="290"/>
     </row>
     <row r="29" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
       <c r="D29" s="35"/>
       <c r="E29" s="36"/>
       <c r="F29" s="34"/>
-      <c r="G29" s="294"/>
-      <c r="H29" s="294"/>
-      <c r="I29" s="294"/>
-      <c r="J29" s="294"/>
-      <c r="K29" s="294"/>
-      <c r="L29" s="294"/>
+      <c r="G29" s="290"/>
+      <c r="H29" s="290"/>
+      <c r="I29" s="290"/>
+      <c r="J29" s="290"/>
+      <c r="K29" s="290"/>
+      <c r="L29" s="290"/>
     </row>
     <row r="30" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
@@ -9382,12 +9354,12 @@
       <c r="D30" s="35"/>
       <c r="E30" s="36"/>
       <c r="F30" s="34"/>
-      <c r="G30" s="294"/>
-      <c r="H30" s="294"/>
-      <c r="I30" s="294"/>
-      <c r="J30" s="294"/>
-      <c r="K30" s="294"/>
-      <c r="L30" s="294"/>
+      <c r="G30" s="290"/>
+      <c r="H30" s="290"/>
+      <c r="I30" s="290"/>
+      <c r="J30" s="290"/>
+      <c r="K30" s="290"/>
+      <c r="L30" s="290"/>
     </row>
     <row r="31" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
@@ -9396,12 +9368,12 @@
       <c r="D31" s="35"/>
       <c r="E31" s="36"/>
       <c r="F31" s="34"/>
-      <c r="G31" s="294"/>
-      <c r="H31" s="294"/>
-      <c r="I31" s="294"/>
-      <c r="J31" s="294"/>
-      <c r="K31" s="294"/>
-      <c r="L31" s="294"/>
+      <c r="G31" s="290"/>
+      <c r="H31" s="290"/>
+      <c r="I31" s="290"/>
+      <c r="J31" s="290"/>
+      <c r="K31" s="290"/>
+      <c r="L31" s="290"/>
     </row>
     <row r="32" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
@@ -9410,12 +9382,12 @@
       <c r="D32" s="35"/>
       <c r="E32" s="36"/>
       <c r="F32" s="34"/>
-      <c r="G32" s="294"/>
-      <c r="H32" s="294"/>
-      <c r="I32" s="294"/>
-      <c r="J32" s="294"/>
-      <c r="K32" s="294"/>
-      <c r="L32" s="294"/>
+      <c r="G32" s="290"/>
+      <c r="H32" s="290"/>
+      <c r="I32" s="290"/>
+      <c r="J32" s="290"/>
+      <c r="K32" s="290"/>
+      <c r="L32" s="290"/>
     </row>
     <row r="33" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
@@ -9424,68 +9396,68 @@
       <c r="D33" s="35"/>
       <c r="E33" s="36"/>
       <c r="F33" s="34"/>
-      <c r="G33" s="294"/>
-      <c r="H33" s="294"/>
-      <c r="I33" s="294"/>
-      <c r="J33" s="294"/>
-      <c r="K33" s="294"/>
-      <c r="L33" s="294"/>
+      <c r="G33" s="290"/>
+      <c r="H33" s="290"/>
+      <c r="I33" s="290"/>
+      <c r="J33" s="290"/>
+      <c r="K33" s="290"/>
+      <c r="L33" s="290"/>
     </row>
     <row r="34" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
+      <c r="A34" s="34"/>
+      <c r="B34" s="34"/>
+      <c r="C34" s="34"/>
       <c r="D34" s="35"/>
       <c r="E34" s="36"/>
       <c r="F34" s="34"/>
-      <c r="G34" s="294"/>
-      <c r="H34" s="294"/>
-      <c r="I34" s="294"/>
-      <c r="J34" s="294"/>
-      <c r="K34" s="294"/>
-      <c r="L34" s="294"/>
+      <c r="G34" s="290"/>
+      <c r="H34" s="290"/>
+      <c r="I34" s="290"/>
+      <c r="J34" s="290"/>
+      <c r="K34" s="290"/>
+      <c r="L34" s="290"/>
     </row>
     <row r="35" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="34"/>
-      <c r="B35" s="34"/>
-      <c r="C35" s="34"/>
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
       <c r="D35" s="35"/>
       <c r="E35" s="36"/>
       <c r="F35" s="34"/>
-      <c r="G35" s="294"/>
-      <c r="H35" s="294"/>
-      <c r="I35" s="294"/>
-      <c r="J35" s="294"/>
-      <c r="K35" s="294"/>
-      <c r="L35" s="294"/>
+      <c r="G35" s="290"/>
+      <c r="H35" s="290"/>
+      <c r="I35" s="290"/>
+      <c r="J35" s="290"/>
+      <c r="K35" s="290"/>
+      <c r="L35" s="290"/>
     </row>
     <row r="36" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
       <c r="D36" s="35"/>
       <c r="E36" s="36"/>
       <c r="F36" s="34"/>
-      <c r="G36" s="294"/>
-      <c r="H36" s="294"/>
-      <c r="I36" s="294"/>
-      <c r="J36" s="294"/>
-      <c r="K36" s="294"/>
-      <c r="L36" s="294"/>
+      <c r="G36" s="290"/>
+      <c r="H36" s="290"/>
+      <c r="I36" s="290"/>
+      <c r="J36" s="290"/>
+      <c r="K36" s="290"/>
+      <c r="L36" s="290"/>
     </row>
     <row r="37" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
       <c r="D37" s="35"/>
       <c r="E37" s="36"/>
       <c r="F37" s="34"/>
-      <c r="G37" s="294"/>
-      <c r="H37" s="294"/>
-      <c r="I37" s="294"/>
-      <c r="J37" s="294"/>
-      <c r="K37" s="294"/>
-      <c r="L37" s="294"/>
+      <c r="G37" s="290"/>
+      <c r="H37" s="290"/>
+      <c r="I37" s="290"/>
+      <c r="J37" s="290"/>
+      <c r="K37" s="290"/>
+      <c r="L37" s="290"/>
     </row>
     <row r="38" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
@@ -9494,26 +9466,26 @@
       <c r="D38" s="35"/>
       <c r="E38" s="36"/>
       <c r="F38" s="34"/>
-      <c r="G38" s="294"/>
-      <c r="H38" s="294"/>
-      <c r="I38" s="294"/>
-      <c r="J38" s="294"/>
-      <c r="K38" s="294"/>
-      <c r="L38" s="294"/>
+      <c r="G38" s="290"/>
+      <c r="H38" s="290"/>
+      <c r="I38" s="290"/>
+      <c r="J38" s="290"/>
+      <c r="K38" s="290"/>
+      <c r="L38" s="290"/>
     </row>
     <row r="39" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
+      <c r="A39" s="7"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
       <c r="D39" s="35"/>
       <c r="E39" s="36"/>
       <c r="F39" s="34"/>
-      <c r="G39" s="294"/>
-      <c r="H39" s="294"/>
-      <c r="I39" s="294"/>
-      <c r="J39" s="294"/>
-      <c r="K39" s="294"/>
-      <c r="L39" s="294"/>
+      <c r="G39" s="290"/>
+      <c r="H39" s="290"/>
+      <c r="I39" s="290"/>
+      <c r="J39" s="290"/>
+      <c r="K39" s="290"/>
+      <c r="L39" s="290"/>
     </row>
     <row r="40" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
@@ -9522,75 +9494,61 @@
       <c r="D40" s="35"/>
       <c r="E40" s="36"/>
       <c r="F40" s="34"/>
-      <c r="G40" s="294"/>
-      <c r="H40" s="294"/>
-      <c r="I40" s="294"/>
-      <c r="J40" s="294"/>
-      <c r="K40" s="294"/>
-      <c r="L40" s="294"/>
-    </row>
-    <row r="41" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="G40" s="290"/>
+      <c r="H40" s="290"/>
+      <c r="I40" s="290"/>
+      <c r="J40" s="290"/>
+      <c r="K40" s="290"/>
+      <c r="L40" s="290"/>
+    </row>
+    <row r="41" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
       <c r="D41" s="35"/>
       <c r="E41" s="36"/>
       <c r="F41" s="34"/>
-      <c r="G41" s="294"/>
-      <c r="H41" s="294"/>
-      <c r="I41" s="294"/>
-      <c r="J41" s="294"/>
-      <c r="K41" s="294"/>
-      <c r="L41" s="294"/>
-    </row>
-    <row r="42" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="7"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="35"/>
-      <c r="E42" s="36"/>
-      <c r="F42" s="34"/>
-      <c r="G42" s="294"/>
-      <c r="H42" s="294"/>
-      <c r="I42" s="294"/>
-      <c r="J42" s="294"/>
-      <c r="K42" s="294"/>
-      <c r="L42" s="294"/>
+      <c r="G41" s="290"/>
+      <c r="H41" s="290"/>
+      <c r="I41" s="290"/>
+      <c r="J41" s="290"/>
+      <c r="K41" s="290"/>
+      <c r="L41" s="290"/>
     </row>
   </sheetData>
-  <mergeCells count="40">
+  <mergeCells count="39">
+    <mergeCell ref="J9:L9"/>
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="J11:L11"/>
     <mergeCell ref="J12:L12"/>
-    <mergeCell ref="J13:L13"/>
     <mergeCell ref="A1:D2"/>
-    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="J8:L8"/>
     <mergeCell ref="J4:L4"/>
     <mergeCell ref="J5:L5"/>
     <mergeCell ref="J6:L6"/>
     <mergeCell ref="J7:L7"/>
-    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="G34:L34"/>
     <mergeCell ref="G35:L35"/>
-    <mergeCell ref="G36:L36"/>
+    <mergeCell ref="G26:L26"/>
     <mergeCell ref="G27:L27"/>
     <mergeCell ref="G28:L28"/>
     <mergeCell ref="G29:L29"/>
     <mergeCell ref="G30:L30"/>
     <mergeCell ref="G31:L31"/>
-    <mergeCell ref="G32:L32"/>
+    <mergeCell ref="G22:L22"/>
     <mergeCell ref="G23:L23"/>
     <mergeCell ref="G24:L24"/>
-    <mergeCell ref="G25:L25"/>
+    <mergeCell ref="G32:L32"/>
     <mergeCell ref="G33:L33"/>
-    <mergeCell ref="G34:L34"/>
-    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="G38:L38"/>
     <mergeCell ref="G39:L39"/>
     <mergeCell ref="G40:L40"/>
     <mergeCell ref="G41:L41"/>
-    <mergeCell ref="G42:L42"/>
+    <mergeCell ref="G36:L36"/>
     <mergeCell ref="G37:L37"/>
-    <mergeCell ref="G38:L38"/>
-    <mergeCell ref="G26:L26"/>
+    <mergeCell ref="G25:L25"/>
+    <mergeCell ref="G14:L14"/>
     <mergeCell ref="G15:L15"/>
     <mergeCell ref="G16:L16"/>
     <mergeCell ref="G17:L17"/>
@@ -9598,7 +9556,6 @@
     <mergeCell ref="G19:L19"/>
     <mergeCell ref="G20:L20"/>
     <mergeCell ref="G21:L21"/>
-    <mergeCell ref="G22:L22"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F2">
@@ -9634,10 +9591,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="284" t="s">
+      <c r="A1" s="280" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="284"/>
+      <c r="B1" s="280"/>
       <c r="C1" s="46" t="s">
         <v>1</v>
       </c>
@@ -9668,8 +9625,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="284"/>
-      <c r="B2" s="284"/>
+      <c r="A2" s="280"/>
+      <c r="B2" s="280"/>
       <c r="C2" s="46" t="s">
         <v>7</v>
       </c>
@@ -9700,16 +9657,16 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="343"/>
-      <c r="B3" s="344"/>
-      <c r="C3" s="344"/>
-      <c r="D3" s="344"/>
-      <c r="E3" s="344"/>
-      <c r="F3" s="344"/>
-      <c r="G3" s="344"/>
-      <c r="H3" s="344"/>
-      <c r="I3" s="344"/>
-      <c r="J3" s="345"/>
+      <c r="A3" s="336"/>
+      <c r="B3" s="337"/>
+      <c r="C3" s="337"/>
+      <c r="D3" s="337"/>
+      <c r="E3" s="337"/>
+      <c r="F3" s="337"/>
+      <c r="G3" s="337"/>
+      <c r="H3" s="337"/>
+      <c r="I3" s="337"/>
+      <c r="J3" s="338"/>
     </row>
     <row r="4" spans="1:10" s="45" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="66" t="s">
@@ -9724,16 +9681,16 @@
       <c r="D4" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="339" t="s">
+      <c r="E4" s="332" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="339"/>
-      <c r="G4" s="340" t="s">
+      <c r="F4" s="332"/>
+      <c r="G4" s="333" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="341"/>
-      <c r="I4" s="341"/>
-      <c r="J4" s="342"/>
+      <c r="H4" s="334"/>
+      <c r="I4" s="334"/>
+      <c r="J4" s="335"/>
     </row>
     <row r="5" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
@@ -9860,336 +9817,336 @@
       <c r="B15" s="35"/>
       <c r="C15" s="36"/>
       <c r="D15" s="34"/>
-      <c r="E15" s="294"/>
-      <c r="F15" s="294"/>
-      <c r="G15" s="294"/>
-      <c r="H15" s="294"/>
-      <c r="I15" s="294"/>
-      <c r="J15" s="294"/>
+      <c r="E15" s="290"/>
+      <c r="F15" s="290"/>
+      <c r="G15" s="290"/>
+      <c r="H15" s="290"/>
+      <c r="I15" s="290"/>
+      <c r="J15" s="290"/>
     </row>
     <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="35"/>
       <c r="C16" s="36"/>
       <c r="D16" s="34"/>
-      <c r="E16" s="294"/>
-      <c r="F16" s="294"/>
-      <c r="G16" s="294"/>
-      <c r="H16" s="294"/>
-      <c r="I16" s="294"/>
-      <c r="J16" s="294"/>
+      <c r="E16" s="290"/>
+      <c r="F16" s="290"/>
+      <c r="G16" s="290"/>
+      <c r="H16" s="290"/>
+      <c r="I16" s="290"/>
+      <c r="J16" s="290"/>
     </row>
     <row r="17" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="35"/>
       <c r="C17" s="36"/>
       <c r="D17" s="34"/>
-      <c r="E17" s="294"/>
-      <c r="F17" s="294"/>
-      <c r="G17" s="294"/>
-      <c r="H17" s="294"/>
-      <c r="I17" s="294"/>
-      <c r="J17" s="294"/>
+      <c r="E17" s="290"/>
+      <c r="F17" s="290"/>
+      <c r="G17" s="290"/>
+      <c r="H17" s="290"/>
+      <c r="I17" s="290"/>
+      <c r="J17" s="290"/>
     </row>
     <row r="18" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="35"/>
       <c r="C18" s="36"/>
       <c r="D18" s="34"/>
-      <c r="E18" s="294"/>
-      <c r="F18" s="294"/>
-      <c r="G18" s="294"/>
-      <c r="H18" s="294"/>
-      <c r="I18" s="294"/>
-      <c r="J18" s="294"/>
+      <c r="E18" s="290"/>
+      <c r="F18" s="290"/>
+      <c r="G18" s="290"/>
+      <c r="H18" s="290"/>
+      <c r="I18" s="290"/>
+      <c r="J18" s="290"/>
     </row>
     <row r="19" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="35"/>
       <c r="C19" s="36"/>
       <c r="D19" s="34"/>
-      <c r="E19" s="294"/>
-      <c r="F19" s="294"/>
-      <c r="G19" s="294"/>
-      <c r="H19" s="294"/>
-      <c r="I19" s="294"/>
-      <c r="J19" s="294"/>
+      <c r="E19" s="290"/>
+      <c r="F19" s="290"/>
+      <c r="G19" s="290"/>
+      <c r="H19" s="290"/>
+      <c r="I19" s="290"/>
+      <c r="J19" s="290"/>
     </row>
     <row r="20" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="35"/>
       <c r="C20" s="36"/>
       <c r="D20" s="34"/>
-      <c r="E20" s="294"/>
-      <c r="F20" s="294"/>
-      <c r="G20" s="294"/>
-      <c r="H20" s="294"/>
-      <c r="I20" s="294"/>
-      <c r="J20" s="294"/>
+      <c r="E20" s="290"/>
+      <c r="F20" s="290"/>
+      <c r="G20" s="290"/>
+      <c r="H20" s="290"/>
+      <c r="I20" s="290"/>
+      <c r="J20" s="290"/>
     </row>
     <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="35"/>
       <c r="C21" s="36"/>
       <c r="D21" s="34"/>
-      <c r="E21" s="294"/>
-      <c r="F21" s="294"/>
-      <c r="G21" s="294"/>
-      <c r="H21" s="294"/>
-      <c r="I21" s="294"/>
-      <c r="J21" s="294"/>
+      <c r="E21" s="290"/>
+      <c r="F21" s="290"/>
+      <c r="G21" s="290"/>
+      <c r="H21" s="290"/>
+      <c r="I21" s="290"/>
+      <c r="J21" s="290"/>
     </row>
     <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="35"/>
       <c r="C22" s="36"/>
       <c r="D22" s="34"/>
-      <c r="E22" s="294"/>
-      <c r="F22" s="294"/>
-      <c r="G22" s="294"/>
-      <c r="H22" s="294"/>
-      <c r="I22" s="294"/>
-      <c r="J22" s="294"/>
+      <c r="E22" s="290"/>
+      <c r="F22" s="290"/>
+      <c r="G22" s="290"/>
+      <c r="H22" s="290"/>
+      <c r="I22" s="290"/>
+      <c r="J22" s="290"/>
     </row>
     <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="35"/>
       <c r="C23" s="36"/>
       <c r="D23" s="34"/>
-      <c r="E23" s="294"/>
-      <c r="F23" s="294"/>
-      <c r="G23" s="294"/>
-      <c r="H23" s="294"/>
-      <c r="I23" s="294"/>
-      <c r="J23" s="294"/>
+      <c r="E23" s="290"/>
+      <c r="F23" s="290"/>
+      <c r="G23" s="290"/>
+      <c r="H23" s="290"/>
+      <c r="I23" s="290"/>
+      <c r="J23" s="290"/>
     </row>
     <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="35"/>
       <c r="C24" s="36"/>
       <c r="D24" s="34"/>
-      <c r="E24" s="294"/>
-      <c r="F24" s="294"/>
-      <c r="G24" s="294"/>
-      <c r="H24" s="294"/>
-      <c r="I24" s="294"/>
-      <c r="J24" s="294"/>
+      <c r="E24" s="290"/>
+      <c r="F24" s="290"/>
+      <c r="G24" s="290"/>
+      <c r="H24" s="290"/>
+      <c r="I24" s="290"/>
+      <c r="J24" s="290"/>
     </row>
     <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A25" s="34"/>
       <c r="B25" s="35"/>
       <c r="C25" s="36"/>
       <c r="D25" s="34"/>
-      <c r="E25" s="294"/>
-      <c r="F25" s="294"/>
-      <c r="G25" s="294"/>
-      <c r="H25" s="294"/>
-      <c r="I25" s="294"/>
-      <c r="J25" s="294"/>
+      <c r="E25" s="290"/>
+      <c r="F25" s="290"/>
+      <c r="G25" s="290"/>
+      <c r="H25" s="290"/>
+      <c r="I25" s="290"/>
+      <c r="J25" s="290"/>
     </row>
     <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="35"/>
       <c r="C26" s="36"/>
       <c r="D26" s="34"/>
-      <c r="E26" s="294"/>
-      <c r="F26" s="294"/>
-      <c r="G26" s="294"/>
-      <c r="H26" s="294"/>
-      <c r="I26" s="294"/>
-      <c r="J26" s="294"/>
+      <c r="E26" s="290"/>
+      <c r="F26" s="290"/>
+      <c r="G26" s="290"/>
+      <c r="H26" s="290"/>
+      <c r="I26" s="290"/>
+      <c r="J26" s="290"/>
     </row>
     <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="35"/>
       <c r="C27" s="36"/>
       <c r="D27" s="34"/>
-      <c r="E27" s="294"/>
-      <c r="F27" s="294"/>
-      <c r="G27" s="294"/>
-      <c r="H27" s="294"/>
-      <c r="I27" s="294"/>
-      <c r="J27" s="294"/>
+      <c r="E27" s="290"/>
+      <c r="F27" s="290"/>
+      <c r="G27" s="290"/>
+      <c r="H27" s="290"/>
+      <c r="I27" s="290"/>
+      <c r="J27" s="290"/>
     </row>
     <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="35"/>
       <c r="C28" s="36"/>
       <c r="D28" s="34"/>
-      <c r="E28" s="294"/>
-      <c r="F28" s="294"/>
-      <c r="G28" s="294"/>
-      <c r="H28" s="294"/>
-      <c r="I28" s="294"/>
-      <c r="J28" s="294"/>
+      <c r="E28" s="290"/>
+      <c r="F28" s="290"/>
+      <c r="G28" s="290"/>
+      <c r="H28" s="290"/>
+      <c r="I28" s="290"/>
+      <c r="J28" s="290"/>
     </row>
     <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="35"/>
       <c r="C29" s="36"/>
       <c r="D29" s="34"/>
-      <c r="E29" s="294"/>
-      <c r="F29" s="294"/>
-      <c r="G29" s="294"/>
-      <c r="H29" s="294"/>
-      <c r="I29" s="294"/>
-      <c r="J29" s="294"/>
+      <c r="E29" s="290"/>
+      <c r="F29" s="290"/>
+      <c r="G29" s="290"/>
+      <c r="H29" s="290"/>
+      <c r="I29" s="290"/>
+      <c r="J29" s="290"/>
     </row>
     <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="35"/>
       <c r="C30" s="36"/>
       <c r="D30" s="34"/>
-      <c r="E30" s="294"/>
-      <c r="F30" s="294"/>
-      <c r="G30" s="294"/>
-      <c r="H30" s="294"/>
-      <c r="I30" s="294"/>
-      <c r="J30" s="294"/>
+      <c r="E30" s="290"/>
+      <c r="F30" s="290"/>
+      <c r="G30" s="290"/>
+      <c r="H30" s="290"/>
+      <c r="I30" s="290"/>
+      <c r="J30" s="290"/>
     </row>
     <row r="31" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="35"/>
       <c r="C31" s="36"/>
       <c r="D31" s="34"/>
-      <c r="E31" s="294"/>
-      <c r="F31" s="294"/>
-      <c r="G31" s="294"/>
-      <c r="H31" s="294"/>
-      <c r="I31" s="294"/>
-      <c r="J31" s="294"/>
+      <c r="E31" s="290"/>
+      <c r="F31" s="290"/>
+      <c r="G31" s="290"/>
+      <c r="H31" s="290"/>
+      <c r="I31" s="290"/>
+      <c r="J31" s="290"/>
     </row>
     <row r="32" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="35"/>
       <c r="C32" s="36"/>
       <c r="D32" s="34"/>
-      <c r="E32" s="294"/>
-      <c r="F32" s="294"/>
-      <c r="G32" s="294"/>
-      <c r="H32" s="294"/>
-      <c r="I32" s="294"/>
-      <c r="J32" s="294"/>
+      <c r="E32" s="290"/>
+      <c r="F32" s="290"/>
+      <c r="G32" s="290"/>
+      <c r="H32" s="290"/>
+      <c r="I32" s="290"/>
+      <c r="J32" s="290"/>
     </row>
     <row r="33" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="35"/>
       <c r="C33" s="36"/>
       <c r="D33" s="34"/>
-      <c r="E33" s="294"/>
-      <c r="F33" s="294"/>
-      <c r="G33" s="294"/>
-      <c r="H33" s="294"/>
-      <c r="I33" s="294"/>
-      <c r="J33" s="294"/>
+      <c r="E33" s="290"/>
+      <c r="F33" s="290"/>
+      <c r="G33" s="290"/>
+      <c r="H33" s="290"/>
+      <c r="I33" s="290"/>
+      <c r="J33" s="290"/>
     </row>
     <row r="34" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="35"/>
       <c r="C34" s="36"/>
       <c r="D34" s="34"/>
-      <c r="E34" s="294"/>
-      <c r="F34" s="294"/>
-      <c r="G34" s="294"/>
-      <c r="H34" s="294"/>
-      <c r="I34" s="294"/>
-      <c r="J34" s="294"/>
+      <c r="E34" s="290"/>
+      <c r="F34" s="290"/>
+      <c r="G34" s="290"/>
+      <c r="H34" s="290"/>
+      <c r="I34" s="290"/>
+      <c r="J34" s="290"/>
     </row>
     <row r="35" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A35" s="34"/>
       <c r="B35" s="35"/>
       <c r="C35" s="36"/>
       <c r="D35" s="34"/>
-      <c r="E35" s="294"/>
-      <c r="F35" s="294"/>
-      <c r="G35" s="294"/>
-      <c r="H35" s="294"/>
-      <c r="I35" s="294"/>
-      <c r="J35" s="294"/>
+      <c r="E35" s="290"/>
+      <c r="F35" s="290"/>
+      <c r="G35" s="290"/>
+      <c r="H35" s="290"/>
+      <c r="I35" s="290"/>
+      <c r="J35" s="290"/>
     </row>
     <row r="36" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="35"/>
       <c r="C36" s="36"/>
       <c r="D36" s="34"/>
-      <c r="E36" s="294"/>
-      <c r="F36" s="294"/>
-      <c r="G36" s="294"/>
-      <c r="H36" s="294"/>
-      <c r="I36" s="294"/>
-      <c r="J36" s="294"/>
+      <c r="E36" s="290"/>
+      <c r="F36" s="290"/>
+      <c r="G36" s="290"/>
+      <c r="H36" s="290"/>
+      <c r="I36" s="290"/>
+      <c r="J36" s="290"/>
     </row>
     <row r="37" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="35"/>
       <c r="C37" s="36"/>
       <c r="D37" s="34"/>
-      <c r="E37" s="294"/>
-      <c r="F37" s="294"/>
-      <c r="G37" s="294"/>
-      <c r="H37" s="294"/>
-      <c r="I37" s="294"/>
-      <c r="J37" s="294"/>
+      <c r="E37" s="290"/>
+      <c r="F37" s="290"/>
+      <c r="G37" s="290"/>
+      <c r="H37" s="290"/>
+      <c r="I37" s="290"/>
+      <c r="J37" s="290"/>
     </row>
     <row r="38" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="35"/>
       <c r="C38" s="36"/>
       <c r="D38" s="34"/>
-      <c r="E38" s="294"/>
-      <c r="F38" s="294"/>
-      <c r="G38" s="294"/>
-      <c r="H38" s="294"/>
-      <c r="I38" s="294"/>
-      <c r="J38" s="294"/>
+      <c r="E38" s="290"/>
+      <c r="F38" s="290"/>
+      <c r="G38" s="290"/>
+      <c r="H38" s="290"/>
+      <c r="I38" s="290"/>
+      <c r="J38" s="290"/>
     </row>
     <row r="39" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="35"/>
       <c r="C39" s="36"/>
       <c r="D39" s="34"/>
-      <c r="E39" s="294"/>
-      <c r="F39" s="294"/>
-      <c r="G39" s="294"/>
-      <c r="H39" s="294"/>
-      <c r="I39" s="294"/>
-      <c r="J39" s="294"/>
+      <c r="E39" s="290"/>
+      <c r="F39" s="290"/>
+      <c r="G39" s="290"/>
+      <c r="H39" s="290"/>
+      <c r="I39" s="290"/>
+      <c r="J39" s="290"/>
     </row>
     <row r="40" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="35"/>
       <c r="C40" s="36"/>
       <c r="D40" s="34"/>
-      <c r="E40" s="294"/>
-      <c r="F40" s="294"/>
-      <c r="G40" s="294"/>
-      <c r="H40" s="294"/>
-      <c r="I40" s="294"/>
-      <c r="J40" s="294"/>
+      <c r="E40" s="290"/>
+      <c r="F40" s="290"/>
+      <c r="G40" s="290"/>
+      <c r="H40" s="290"/>
+      <c r="I40" s="290"/>
+      <c r="J40" s="290"/>
     </row>
     <row r="41" spans="1:10" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="35"/>
       <c r="C41" s="36"/>
       <c r="D41" s="34"/>
-      <c r="E41" s="294"/>
-      <c r="F41" s="294"/>
-      <c r="G41" s="294"/>
-      <c r="H41" s="294"/>
-      <c r="I41" s="294"/>
-      <c r="J41" s="294"/>
+      <c r="E41" s="290"/>
+      <c r="F41" s="290"/>
+      <c r="G41" s="290"/>
+      <c r="H41" s="290"/>
+      <c r="I41" s="290"/>
+      <c r="J41" s="290"/>
     </row>
     <row r="42" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="35"/>
       <c r="C42" s="36"/>
       <c r="D42" s="34"/>
-      <c r="E42" s="294"/>
-      <c r="F42" s="294"/>
-      <c r="G42" s="294"/>
-      <c r="H42" s="294"/>
-      <c r="I42" s="294"/>
-      <c r="J42" s="294"/>
+      <c r="E42" s="290"/>
+      <c r="F42" s="290"/>
+      <c r="G42" s="290"/>
+      <c r="H42" s="290"/>
+      <c r="I42" s="290"/>
+      <c r="J42" s="290"/>
     </row>
   </sheetData>
   <mergeCells count="32">
@@ -10241,8 +10198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S43"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A12" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10269,12 +10226,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="284" t="s">
+      <c r="A1" s="280" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="284"/>
-      <c r="C1" s="284"/>
-      <c r="D1" s="284"/>
+      <c r="B1" s="280"/>
+      <c r="C1" s="280"/>
+      <c r="D1" s="280"/>
       <c r="E1" s="46" t="s">
         <v>1</v>
       </c>
@@ -10312,10 +10269,10 @@
       <c r="S1" s="17"/>
     </row>
     <row r="2" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="284"/>
-      <c r="B2" s="284"/>
-      <c r="C2" s="284"/>
-      <c r="D2" s="284"/>
+      <c r="A2" s="280"/>
+      <c r="B2" s="280"/>
+      <c r="C2" s="280"/>
+      <c r="D2" s="280"/>
       <c r="E2" s="46" t="s">
         <v>7</v>
       </c>
@@ -10353,18 +10310,18 @@
       <c r="S2" s="17"/>
     </row>
     <row r="3" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="343"/>
-      <c r="B3" s="344"/>
-      <c r="C3" s="344"/>
-      <c r="D3" s="344"/>
-      <c r="E3" s="344"/>
-      <c r="F3" s="344"/>
-      <c r="G3" s="344"/>
-      <c r="H3" s="344"/>
-      <c r="I3" s="344"/>
-      <c r="J3" s="344"/>
-      <c r="K3" s="344"/>
-      <c r="L3" s="345"/>
+      <c r="A3" s="336"/>
+      <c r="B3" s="337"/>
+      <c r="C3" s="337"/>
+      <c r="D3" s="337"/>
+      <c r="E3" s="337"/>
+      <c r="F3" s="337"/>
+      <c r="G3" s="337"/>
+      <c r="H3" s="337"/>
+      <c r="I3" s="337"/>
+      <c r="J3" s="337"/>
+      <c r="K3" s="337"/>
+      <c r="L3" s="338"/>
       <c r="M3" s="17"/>
       <c r="N3" s="17"/>
       <c r="O3" s="17"/>
@@ -10377,11 +10334,11 @@
       <c r="A4" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="280" t="s">
-        <v>321</v>
-      </c>
-      <c r="C4" s="280" t="s">
-        <v>322</v>
+      <c r="B4" s="276" t="s">
+        <v>313</v>
+      </c>
+      <c r="C4" s="276" t="s">
+        <v>314</v>
       </c>
       <c r="D4" s="66" t="s">
         <v>46</v>
@@ -10404,12 +10361,12 @@
       <c r="J4" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="K4" s="340" t="s">
+      <c r="K4" s="333" t="s">
         <v>43</v>
       </c>
-      <c r="L4" s="341"/>
-      <c r="M4" s="341"/>
-      <c r="N4" s="342"/>
+      <c r="L4" s="334"/>
+      <c r="M4" s="334"/>
+      <c r="N4" s="335"/>
       <c r="O4" s="66" t="s">
         <v>44</v>
       </c>
@@ -10447,12 +10404,12 @@
       <c r="J5" s="160" t="s">
         <v>223</v>
       </c>
-      <c r="K5" s="346" t="s">
+      <c r="K5" s="339" t="s">
         <v>224</v>
       </c>
-      <c r="L5" s="347"/>
-      <c r="M5" s="347"/>
-      <c r="N5" s="348"/>
+      <c r="L5" s="340"/>
+      <c r="M5" s="340"/>
+      <c r="N5" s="341"/>
       <c r="O5" s="160"/>
       <c r="P5" s="159"/>
       <c r="Q5" s="164" t="s">
@@ -10484,12 +10441,12 @@
       <c r="J6" s="160" t="s">
         <v>227</v>
       </c>
-      <c r="K6" s="349" t="s">
+      <c r="K6" s="342" t="s">
         <v>228</v>
       </c>
-      <c r="L6" s="350"/>
-      <c r="M6" s="350"/>
-      <c r="N6" s="351"/>
+      <c r="L6" s="343"/>
+      <c r="M6" s="343"/>
+      <c r="N6" s="344"/>
       <c r="O6" s="181" t="s">
         <v>230</v>
       </c>
@@ -10521,12 +10478,12 @@
       <c r="J7" s="160" t="s">
         <v>233</v>
       </c>
-      <c r="K7" s="349" t="s">
+      <c r="K7" s="342" t="s">
         <v>249</v>
       </c>
-      <c r="L7" s="350"/>
-      <c r="M7" s="350"/>
-      <c r="N7" s="351"/>
+      <c r="L7" s="343"/>
+      <c r="M7" s="343"/>
+      <c r="N7" s="344"/>
       <c r="O7" s="185" t="s">
         <v>234</v>
       </c>
@@ -10558,12 +10515,12 @@
       <c r="J8" s="160" t="s">
         <v>239</v>
       </c>
-      <c r="K8" s="346" t="s">
+      <c r="K8" s="339" t="s">
         <v>248</v>
       </c>
-      <c r="L8" s="347"/>
-      <c r="M8" s="347"/>
-      <c r="N8" s="348"/>
+      <c r="L8" s="340"/>
+      <c r="M8" s="340"/>
+      <c r="N8" s="341"/>
       <c r="O8" s="153"/>
       <c r="P8" s="153"/>
       <c r="Q8" s="153"/>
@@ -10591,12 +10548,12 @@
       <c r="J9" s="197" t="s">
         <v>254</v>
       </c>
-      <c r="K9" s="352" t="s">
+      <c r="K9" s="345" t="s">
         <v>255</v>
       </c>
-      <c r="L9" s="353"/>
-      <c r="M9" s="353"/>
-      <c r="N9" s="354"/>
+      <c r="L9" s="346"/>
+      <c r="M9" s="346"/>
+      <c r="N9" s="347"/>
       <c r="O9" s="198"/>
       <c r="P9" s="198"/>
       <c r="Q9" s="198"/>
@@ -10624,12 +10581,12 @@
       <c r="J10" s="197" t="s">
         <v>257</v>
       </c>
-      <c r="K10" s="356" t="s">
+      <c r="K10" s="349" t="s">
         <v>258</v>
       </c>
-      <c r="L10" s="357"/>
-      <c r="M10" s="357"/>
-      <c r="N10" s="358"/>
+      <c r="L10" s="350"/>
+      <c r="M10" s="350"/>
+      <c r="N10" s="351"/>
       <c r="O10" s="202" t="s">
         <v>259</v>
       </c>
@@ -10661,12 +10618,12 @@
       <c r="J11" s="197" t="s">
         <v>262</v>
       </c>
-      <c r="K11" s="356" t="s">
+      <c r="K11" s="349" t="s">
         <v>263</v>
       </c>
-      <c r="L11" s="357"/>
-      <c r="M11" s="357"/>
-      <c r="N11" s="358"/>
+      <c r="L11" s="350"/>
+      <c r="M11" s="350"/>
+      <c r="N11" s="351"/>
       <c r="O11" s="205" t="s">
         <v>264</v>
       </c>
@@ -10698,12 +10655,12 @@
       <c r="J12" s="197" t="s">
         <v>267</v>
       </c>
-      <c r="K12" s="356" t="s">
+      <c r="K12" s="349" t="s">
         <v>268</v>
       </c>
-      <c r="L12" s="357"/>
-      <c r="M12" s="357"/>
-      <c r="N12" s="358"/>
+      <c r="L12" s="350"/>
+      <c r="M12" s="350"/>
+      <c r="N12" s="351"/>
       <c r="O12" s="198"/>
       <c r="P12" s="198"/>
       <c r="Q12" s="198"/>
@@ -10735,12 +10692,12 @@
       <c r="J13" s="233" t="s">
         <v>288</v>
       </c>
-      <c r="K13" s="359" t="s">
+      <c r="K13" s="352" t="s">
         <v>282</v>
       </c>
-      <c r="L13" s="360"/>
-      <c r="M13" s="360"/>
-      <c r="N13" s="361"/>
+      <c r="L13" s="353"/>
+      <c r="M13" s="353"/>
+      <c r="N13" s="354"/>
       <c r="O13" s="234" t="s">
         <v>283</v>
       </c>
@@ -10778,12 +10735,12 @@
       <c r="J14" s="258" t="s">
         <v>292</v>
       </c>
-      <c r="K14" s="362" t="s">
+      <c r="K14" s="355" t="s">
         <v>289</v>
       </c>
-      <c r="L14" s="363"/>
-      <c r="M14" s="363"/>
-      <c r="N14" s="364"/>
+      <c r="L14" s="356"/>
+      <c r="M14" s="356"/>
+      <c r="N14" s="357"/>
       <c r="O14" s="259" t="s">
         <v>290</v>
       </c>
@@ -10801,7 +10758,7 @@
         <v>11</v>
       </c>
       <c r="B15" s="264" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C15" s="264">
         <v>51</v>
@@ -10825,17 +10782,17 @@
       <c r="J15" s="270" t="s">
         <v>309</v>
       </c>
-      <c r="K15" s="365" t="s">
+      <c r="K15" s="358" t="s">
+        <v>316</v>
+      </c>
+      <c r="L15" s="359"/>
+      <c r="M15" s="359"/>
+      <c r="N15" s="360"/>
+      <c r="O15" s="271" t="s">
         <v>310</v>
       </c>
-      <c r="L15" s="366"/>
-      <c r="M15" s="366"/>
-      <c r="N15" s="367"/>
-      <c r="O15" s="271" t="s">
+      <c r="P15" s="271" t="s">
         <v>311</v>
-      </c>
-      <c r="P15" s="271" t="s">
-        <v>312</v>
       </c>
       <c r="Q15" s="269" t="s">
         <v>307</v>
@@ -10844,7 +10801,7 @@
         <v>171</v>
       </c>
       <c r="S15" s="268" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="16" spans="1:19" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
@@ -10875,12 +10832,12 @@
       <c r="D17" s="39"/>
       <c r="E17" s="42"/>
       <c r="F17" s="38"/>
-      <c r="G17" s="355"/>
-      <c r="H17" s="355"/>
-      <c r="I17" s="355"/>
-      <c r="J17" s="355"/>
-      <c r="K17" s="355"/>
-      <c r="L17" s="355"/>
+      <c r="G17" s="348"/>
+      <c r="H17" s="348"/>
+      <c r="I17" s="348"/>
+      <c r="J17" s="348"/>
+      <c r="K17" s="348"/>
+      <c r="L17" s="348"/>
     </row>
     <row r="18" spans="1:12" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
@@ -10889,12 +10846,12 @@
       <c r="D18" s="39"/>
       <c r="E18" s="42"/>
       <c r="F18" s="38"/>
-      <c r="G18" s="355"/>
-      <c r="H18" s="355"/>
-      <c r="I18" s="355"/>
-      <c r="J18" s="355"/>
-      <c r="K18" s="355"/>
-      <c r="L18" s="355"/>
+      <c r="G18" s="348"/>
+      <c r="H18" s="348"/>
+      <c r="I18" s="348"/>
+      <c r="J18" s="348"/>
+      <c r="K18" s="348"/>
+      <c r="L18" s="348"/>
     </row>
     <row r="19" spans="1:12" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
@@ -10903,12 +10860,12 @@
       <c r="D19" s="39"/>
       <c r="E19" s="42"/>
       <c r="F19" s="38"/>
-      <c r="G19" s="355"/>
-      <c r="H19" s="355"/>
-      <c r="I19" s="355"/>
-      <c r="J19" s="355"/>
-      <c r="K19" s="355"/>
-      <c r="L19" s="355"/>
+      <c r="G19" s="348"/>
+      <c r="H19" s="348"/>
+      <c r="I19" s="348"/>
+      <c r="J19" s="348"/>
+      <c r="K19" s="348"/>
+      <c r="L19" s="348"/>
     </row>
     <row r="20" spans="1:12" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
@@ -10917,12 +10874,12 @@
       <c r="D20" s="39"/>
       <c r="E20" s="42"/>
       <c r="F20" s="38"/>
-      <c r="G20" s="355"/>
-      <c r="H20" s="355"/>
-      <c r="I20" s="355"/>
-      <c r="J20" s="355"/>
-      <c r="K20" s="355"/>
-      <c r="L20" s="355"/>
+      <c r="G20" s="348"/>
+      <c r="H20" s="348"/>
+      <c r="I20" s="348"/>
+      <c r="J20" s="348"/>
+      <c r="K20" s="348"/>
+      <c r="L20" s="348"/>
     </row>
     <row r="21" spans="1:12" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
@@ -10931,12 +10888,12 @@
       <c r="D21" s="39"/>
       <c r="E21" s="42"/>
       <c r="F21" s="38"/>
-      <c r="G21" s="355"/>
-      <c r="H21" s="355"/>
-      <c r="I21" s="355"/>
-      <c r="J21" s="355"/>
-      <c r="K21" s="355"/>
-      <c r="L21" s="355"/>
+      <c r="G21" s="348"/>
+      <c r="H21" s="348"/>
+      <c r="I21" s="348"/>
+      <c r="J21" s="348"/>
+      <c r="K21" s="348"/>
+      <c r="L21" s="348"/>
     </row>
     <row r="22" spans="1:12" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
@@ -10945,12 +10902,12 @@
       <c r="D22" s="39"/>
       <c r="E22" s="42"/>
       <c r="F22" s="38"/>
-      <c r="G22" s="355"/>
-      <c r="H22" s="355"/>
-      <c r="I22" s="355"/>
-      <c r="J22" s="355"/>
-      <c r="K22" s="355"/>
-      <c r="L22" s="355"/>
+      <c r="G22" s="348"/>
+      <c r="H22" s="348"/>
+      <c r="I22" s="348"/>
+      <c r="J22" s="348"/>
+      <c r="K22" s="348"/>
+      <c r="L22" s="348"/>
     </row>
     <row r="23" spans="1:12" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
@@ -10959,12 +10916,12 @@
       <c r="D23" s="39"/>
       <c r="E23" s="42"/>
       <c r="F23" s="38"/>
-      <c r="G23" s="355"/>
-      <c r="H23" s="355"/>
-      <c r="I23" s="355"/>
-      <c r="J23" s="355"/>
-      <c r="K23" s="355"/>
-      <c r="L23" s="355"/>
+      <c r="G23" s="348"/>
+      <c r="H23" s="348"/>
+      <c r="I23" s="348"/>
+      <c r="J23" s="348"/>
+      <c r="K23" s="348"/>
+      <c r="L23" s="348"/>
     </row>
     <row r="24" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
@@ -10973,12 +10930,12 @@
       <c r="D24" s="35"/>
       <c r="E24" s="36"/>
       <c r="F24" s="34"/>
-      <c r="G24" s="294"/>
-      <c r="H24" s="294"/>
-      <c r="I24" s="294"/>
-      <c r="J24" s="294"/>
-      <c r="K24" s="294"/>
-      <c r="L24" s="294"/>
+      <c r="G24" s="290"/>
+      <c r="H24" s="290"/>
+      <c r="I24" s="290"/>
+      <c r="J24" s="290"/>
+      <c r="K24" s="290"/>
+      <c r="L24" s="290"/>
     </row>
     <row r="25" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
@@ -10987,12 +10944,12 @@
       <c r="D25" s="35"/>
       <c r="E25" s="36"/>
       <c r="F25" s="34"/>
-      <c r="G25" s="294"/>
-      <c r="H25" s="294"/>
-      <c r="I25" s="294"/>
-      <c r="J25" s="294"/>
-      <c r="K25" s="294"/>
-      <c r="L25" s="294"/>
+      <c r="G25" s="290"/>
+      <c r="H25" s="290"/>
+      <c r="I25" s="290"/>
+      <c r="J25" s="290"/>
+      <c r="K25" s="290"/>
+      <c r="L25" s="290"/>
     </row>
     <row r="26" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A26" s="34"/>
@@ -11001,12 +10958,12 @@
       <c r="D26" s="35"/>
       <c r="E26" s="36"/>
       <c r="F26" s="34"/>
-      <c r="G26" s="294"/>
-      <c r="H26" s="294"/>
-      <c r="I26" s="294"/>
-      <c r="J26" s="294"/>
-      <c r="K26" s="294"/>
-      <c r="L26" s="294"/>
+      <c r="G26" s="290"/>
+      <c r="H26" s="290"/>
+      <c r="I26" s="290"/>
+      <c r="J26" s="290"/>
+      <c r="K26" s="290"/>
+      <c r="L26" s="290"/>
     </row>
     <row r="27" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
@@ -11015,12 +10972,12 @@
       <c r="D27" s="35"/>
       <c r="E27" s="36"/>
       <c r="F27" s="34"/>
-      <c r="G27" s="294"/>
-      <c r="H27" s="294"/>
-      <c r="I27" s="294"/>
-      <c r="J27" s="294"/>
-      <c r="K27" s="294"/>
-      <c r="L27" s="294"/>
+      <c r="G27" s="290"/>
+      <c r="H27" s="290"/>
+      <c r="I27" s="290"/>
+      <c r="J27" s="290"/>
+      <c r="K27" s="290"/>
+      <c r="L27" s="290"/>
     </row>
     <row r="28" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
@@ -11029,12 +10986,12 @@
       <c r="D28" s="35"/>
       <c r="E28" s="36"/>
       <c r="F28" s="34"/>
-      <c r="G28" s="294"/>
-      <c r="H28" s="294"/>
-      <c r="I28" s="294"/>
-      <c r="J28" s="294"/>
-      <c r="K28" s="294"/>
-      <c r="L28" s="294"/>
+      <c r="G28" s="290"/>
+      <c r="H28" s="290"/>
+      <c r="I28" s="290"/>
+      <c r="J28" s="290"/>
+      <c r="K28" s="290"/>
+      <c r="L28" s="290"/>
     </row>
     <row r="29" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
@@ -11043,12 +11000,12 @@
       <c r="D29" s="35"/>
       <c r="E29" s="36"/>
       <c r="F29" s="34"/>
-      <c r="G29" s="294"/>
-      <c r="H29" s="294"/>
-      <c r="I29" s="294"/>
-      <c r="J29" s="294"/>
-      <c r="K29" s="294"/>
-      <c r="L29" s="294"/>
+      <c r="G29" s="290"/>
+      <c r="H29" s="290"/>
+      <c r="I29" s="290"/>
+      <c r="J29" s="290"/>
+      <c r="K29" s="290"/>
+      <c r="L29" s="290"/>
     </row>
     <row r="30" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
@@ -11057,12 +11014,12 @@
       <c r="D30" s="35"/>
       <c r="E30" s="36"/>
       <c r="F30" s="34"/>
-      <c r="G30" s="294"/>
-      <c r="H30" s="294"/>
-      <c r="I30" s="294"/>
-      <c r="J30" s="294"/>
-      <c r="K30" s="294"/>
-      <c r="L30" s="294"/>
+      <c r="G30" s="290"/>
+      <c r="H30" s="290"/>
+      <c r="I30" s="290"/>
+      <c r="J30" s="290"/>
+      <c r="K30" s="290"/>
+      <c r="L30" s="290"/>
     </row>
     <row r="31" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
@@ -11071,12 +11028,12 @@
       <c r="D31" s="35"/>
       <c r="E31" s="36"/>
       <c r="F31" s="34"/>
-      <c r="G31" s="294"/>
-      <c r="H31" s="294"/>
-      <c r="I31" s="294"/>
-      <c r="J31" s="294"/>
-      <c r="K31" s="294"/>
-      <c r="L31" s="294"/>
+      <c r="G31" s="290"/>
+      <c r="H31" s="290"/>
+      <c r="I31" s="290"/>
+      <c r="J31" s="290"/>
+      <c r="K31" s="290"/>
+      <c r="L31" s="290"/>
     </row>
     <row r="32" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
@@ -11085,12 +11042,12 @@
       <c r="D32" s="35"/>
       <c r="E32" s="36"/>
       <c r="F32" s="34"/>
-      <c r="G32" s="294"/>
-      <c r="H32" s="294"/>
-      <c r="I32" s="294"/>
-      <c r="J32" s="294"/>
-      <c r="K32" s="294"/>
-      <c r="L32" s="294"/>
+      <c r="G32" s="290"/>
+      <c r="H32" s="290"/>
+      <c r="I32" s="290"/>
+      <c r="J32" s="290"/>
+      <c r="K32" s="290"/>
+      <c r="L32" s="290"/>
     </row>
     <row r="33" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
@@ -11099,12 +11056,12 @@
       <c r="D33" s="35"/>
       <c r="E33" s="36"/>
       <c r="F33" s="34"/>
-      <c r="G33" s="294"/>
-      <c r="H33" s="294"/>
-      <c r="I33" s="294"/>
-      <c r="J33" s="294"/>
-      <c r="K33" s="294"/>
-      <c r="L33" s="294"/>
+      <c r="G33" s="290"/>
+      <c r="H33" s="290"/>
+      <c r="I33" s="290"/>
+      <c r="J33" s="290"/>
+      <c r="K33" s="290"/>
+      <c r="L33" s="290"/>
     </row>
     <row r="34" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
@@ -11113,12 +11070,12 @@
       <c r="D34" s="35"/>
       <c r="E34" s="36"/>
       <c r="F34" s="34"/>
-      <c r="G34" s="294"/>
-      <c r="H34" s="294"/>
-      <c r="I34" s="294"/>
-      <c r="J34" s="294"/>
-      <c r="K34" s="294"/>
-      <c r="L34" s="294"/>
+      <c r="G34" s="290"/>
+      <c r="H34" s="290"/>
+      <c r="I34" s="290"/>
+      <c r="J34" s="290"/>
+      <c r="K34" s="290"/>
+      <c r="L34" s="290"/>
     </row>
     <row r="35" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
@@ -11127,12 +11084,12 @@
       <c r="D35" s="35"/>
       <c r="E35" s="36"/>
       <c r="F35" s="34"/>
-      <c r="G35" s="294"/>
-      <c r="H35" s="294"/>
-      <c r="I35" s="294"/>
-      <c r="J35" s="294"/>
-      <c r="K35" s="294"/>
-      <c r="L35" s="294"/>
+      <c r="G35" s="290"/>
+      <c r="H35" s="290"/>
+      <c r="I35" s="290"/>
+      <c r="J35" s="290"/>
+      <c r="K35" s="290"/>
+      <c r="L35" s="290"/>
     </row>
     <row r="36" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A36" s="34"/>
@@ -11141,12 +11098,12 @@
       <c r="D36" s="35"/>
       <c r="E36" s="36"/>
       <c r="F36" s="34"/>
-      <c r="G36" s="294"/>
-      <c r="H36" s="294"/>
-      <c r="I36" s="294"/>
-      <c r="J36" s="294"/>
-      <c r="K36" s="294"/>
-      <c r="L36" s="294"/>
+      <c r="G36" s="290"/>
+      <c r="H36" s="290"/>
+      <c r="I36" s="290"/>
+      <c r="J36" s="290"/>
+      <c r="K36" s="290"/>
+      <c r="L36" s="290"/>
     </row>
     <row r="37" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
@@ -11155,12 +11112,12 @@
       <c r="D37" s="35"/>
       <c r="E37" s="36"/>
       <c r="F37" s="34"/>
-      <c r="G37" s="294"/>
-      <c r="H37" s="294"/>
-      <c r="I37" s="294"/>
-      <c r="J37" s="294"/>
-      <c r="K37" s="294"/>
-      <c r="L37" s="294"/>
+      <c r="G37" s="290"/>
+      <c r="H37" s="290"/>
+      <c r="I37" s="290"/>
+      <c r="J37" s="290"/>
+      <c r="K37" s="290"/>
+      <c r="L37" s="290"/>
     </row>
     <row r="38" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
@@ -11169,12 +11126,12 @@
       <c r="D38" s="35"/>
       <c r="E38" s="36"/>
       <c r="F38" s="34"/>
-      <c r="G38" s="294"/>
-      <c r="H38" s="294"/>
-      <c r="I38" s="294"/>
-      <c r="J38" s="294"/>
-      <c r="K38" s="294"/>
-      <c r="L38" s="294"/>
+      <c r="G38" s="290"/>
+      <c r="H38" s="290"/>
+      <c r="I38" s="290"/>
+      <c r="J38" s="290"/>
+      <c r="K38" s="290"/>
+      <c r="L38" s="290"/>
     </row>
     <row r="39" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
@@ -11183,12 +11140,12 @@
       <c r="D39" s="35"/>
       <c r="E39" s="36"/>
       <c r="F39" s="34"/>
-      <c r="G39" s="294"/>
-      <c r="H39" s="294"/>
-      <c r="I39" s="294"/>
-      <c r="J39" s="294"/>
-      <c r="K39" s="294"/>
-      <c r="L39" s="294"/>
+      <c r="G39" s="290"/>
+      <c r="H39" s="290"/>
+      <c r="I39" s="290"/>
+      <c r="J39" s="290"/>
+      <c r="K39" s="290"/>
+      <c r="L39" s="290"/>
     </row>
     <row r="40" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
@@ -11197,12 +11154,12 @@
       <c r="D40" s="35"/>
       <c r="E40" s="36"/>
       <c r="F40" s="34"/>
-      <c r="G40" s="294"/>
-      <c r="H40" s="294"/>
-      <c r="I40" s="294"/>
-      <c r="J40" s="294"/>
-      <c r="K40" s="294"/>
-      <c r="L40" s="294"/>
+      <c r="G40" s="290"/>
+      <c r="H40" s="290"/>
+      <c r="I40" s="290"/>
+      <c r="J40" s="290"/>
+      <c r="K40" s="290"/>
+      <c r="L40" s="290"/>
     </row>
     <row r="41" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
@@ -11211,12 +11168,12 @@
       <c r="D41" s="35"/>
       <c r="E41" s="36"/>
       <c r="F41" s="34"/>
-      <c r="G41" s="294"/>
-      <c r="H41" s="294"/>
-      <c r="I41" s="294"/>
-      <c r="J41" s="294"/>
-      <c r="K41" s="294"/>
-      <c r="L41" s="294"/>
+      <c r="G41" s="290"/>
+      <c r="H41" s="290"/>
+      <c r="I41" s="290"/>
+      <c r="J41" s="290"/>
+      <c r="K41" s="290"/>
+      <c r="L41" s="290"/>
     </row>
     <row r="42" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
@@ -11225,12 +11182,12 @@
       <c r="D42" s="35"/>
       <c r="E42" s="36"/>
       <c r="F42" s="34"/>
-      <c r="G42" s="294"/>
-      <c r="H42" s="294"/>
-      <c r="I42" s="294"/>
-      <c r="J42" s="294"/>
-      <c r="K42" s="294"/>
-      <c r="L42" s="294"/>
+      <c r="G42" s="290"/>
+      <c r="H42" s="290"/>
+      <c r="I42" s="290"/>
+      <c r="J42" s="290"/>
+      <c r="K42" s="290"/>
+      <c r="L42" s="290"/>
     </row>
     <row r="43" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
@@ -11239,12 +11196,12 @@
       <c r="D43" s="35"/>
       <c r="E43" s="36"/>
       <c r="F43" s="34"/>
-      <c r="G43" s="294"/>
-      <c r="H43" s="294"/>
-      <c r="I43" s="294"/>
-      <c r="J43" s="294"/>
-      <c r="K43" s="294"/>
-      <c r="L43" s="294"/>
+      <c r="G43" s="290"/>
+      <c r="H43" s="290"/>
+      <c r="I43" s="290"/>
+      <c r="J43" s="290"/>
+      <c r="K43" s="290"/>
+      <c r="L43" s="290"/>
     </row>
   </sheetData>
   <mergeCells count="41">
@@ -11315,8 +11272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L59"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37:K37"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A31" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -11335,11 +11292,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="284" t="s">
+      <c r="A1" s="280" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="284"/>
-      <c r="C1" s="284"/>
+      <c r="B1" s="280"/>
+      <c r="C1" s="280"/>
       <c r="D1" s="46" t="s">
         <v>1</v>
       </c>
@@ -11370,9 +11327,9 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="284"/>
-      <c r="B2" s="284"/>
-      <c r="C2" s="284"/>
+      <c r="A2" s="280"/>
+      <c r="B2" s="280"/>
+      <c r="C2" s="280"/>
       <c r="D2" s="46" t="s">
         <v>7</v>
       </c>
@@ -11915,22 +11872,22 @@
       <c r="J36" s="251"/>
       <c r="K36" s="251"/>
     </row>
-    <row r="37" spans="1:12" s="272" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" s="272" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="273" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B37" s="274"/>
-      <c r="C37" s="368" t="s">
-        <v>320</v>
-      </c>
-      <c r="D37" s="368"/>
-      <c r="E37" s="368"/>
-      <c r="F37" s="368"/>
-      <c r="G37" s="368"/>
-      <c r="H37" s="368"/>
-      <c r="I37" s="368"/>
-      <c r="J37" s="368"/>
-      <c r="K37" s="368"/>
+      <c r="C37" s="361" t="s">
+        <v>318</v>
+      </c>
+      <c r="D37" s="361"/>
+      <c r="E37" s="361"/>
+      <c r="F37" s="361"/>
+      <c r="G37" s="361"/>
+      <c r="H37" s="361"/>
+      <c r="I37" s="361"/>
+      <c r="J37" s="361"/>
+      <c r="K37" s="361"/>
     </row>
     <row r="38" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A38" s="167" t="s">
@@ -12019,12 +11976,12 @@
       <c r="C43" s="39"/>
       <c r="D43" s="42"/>
       <c r="E43" s="38"/>
-      <c r="F43" s="355"/>
-      <c r="G43" s="355"/>
-      <c r="H43" s="355"/>
-      <c r="I43" s="355"/>
-      <c r="J43" s="355"/>
-      <c r="K43" s="355"/>
+      <c r="F43" s="348"/>
+      <c r="G43" s="348"/>
+      <c r="H43" s="348"/>
+      <c r="I43" s="348"/>
+      <c r="J43" s="348"/>
+      <c r="K43" s="348"/>
       <c r="L43" s="17"/>
     </row>
     <row r="44" spans="1:12" s="199" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
@@ -12050,12 +12007,12 @@
       <c r="C45" s="39"/>
       <c r="D45" s="42"/>
       <c r="E45" s="38"/>
-      <c r="F45" s="355"/>
-      <c r="G45" s="355"/>
-      <c r="H45" s="355"/>
-      <c r="I45" s="355"/>
-      <c r="J45" s="355"/>
-      <c r="K45" s="355"/>
+      <c r="F45" s="348"/>
+      <c r="G45" s="348"/>
+      <c r="H45" s="348"/>
+      <c r="I45" s="348"/>
+      <c r="J45" s="348"/>
+      <c r="K45" s="348"/>
       <c r="L45" s="17"/>
     </row>
     <row r="46" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -12066,12 +12023,12 @@
       <c r="C46" s="39"/>
       <c r="D46" s="42"/>
       <c r="E46" s="38"/>
-      <c r="F46" s="355"/>
-      <c r="G46" s="355"/>
-      <c r="H46" s="355"/>
-      <c r="I46" s="355"/>
-      <c r="J46" s="355"/>
-      <c r="K46" s="355"/>
+      <c r="F46" s="348"/>
+      <c r="G46" s="348"/>
+      <c r="H46" s="348"/>
+      <c r="I46" s="348"/>
+      <c r="J46" s="348"/>
+      <c r="K46" s="348"/>
       <c r="L46" s="17"/>
     </row>
     <row r="47" spans="1:12" s="199" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -12082,19 +12039,13 @@
         <v>275</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="17"/>
-      <c r="B48" s="17"/>
-      <c r="C48" s="17"/>
-      <c r="D48" s="17"/>
-      <c r="E48" s="17"/>
-      <c r="F48" s="17"/>
-      <c r="G48" s="17"/>
-      <c r="H48" s="17"/>
-      <c r="I48" s="17"/>
-      <c r="J48" s="17"/>
-      <c r="K48" s="17"/>
-      <c r="L48" s="17"/>
+    <row r="48" spans="1:12" s="272" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="272" t="s">
+        <v>319</v>
+      </c>
+      <c r="C48" s="272" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="49" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="17"/>
@@ -12293,11 +12244,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="284" t="s">
+      <c r="A1" s="280" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="284"/>
-      <c r="C1" s="284"/>
+      <c r="B1" s="280"/>
+      <c r="C1" s="280"/>
       <c r="D1" s="46" t="s">
         <v>1</v>
       </c>
@@ -12320,9 +12271,9 @@
       <c r="K1" s="15"/>
     </row>
     <row r="2" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="284"/>
-      <c r="B2" s="284"/>
-      <c r="C2" s="284"/>
+      <c r="A2" s="280"/>
+      <c r="B2" s="280"/>
+      <c r="C2" s="280"/>
       <c r="D2" s="46" t="s">
         <v>7</v>
       </c>
@@ -12692,12 +12643,12 @@
       <c r="C28" s="39"/>
       <c r="D28" s="42"/>
       <c r="E28" s="38"/>
-      <c r="F28" s="355"/>
-      <c r="G28" s="355"/>
-      <c r="H28" s="355"/>
-      <c r="I28" s="355"/>
-      <c r="J28" s="355"/>
-      <c r="K28" s="355"/>
+      <c r="F28" s="348"/>
+      <c r="G28" s="348"/>
+      <c r="H28" s="348"/>
+      <c r="I28" s="348"/>
+      <c r="J28" s="348"/>
+      <c r="K28" s="348"/>
       <c r="L28" s="17"/>
     </row>
     <row r="29" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
@@ -12706,12 +12657,12 @@
       <c r="C29" s="39"/>
       <c r="D29" s="42"/>
       <c r="E29" s="38"/>
-      <c r="F29" s="355"/>
-      <c r="G29" s="355"/>
-      <c r="H29" s="355"/>
-      <c r="I29" s="355"/>
-      <c r="J29" s="355"/>
-      <c r="K29" s="355"/>
+      <c r="F29" s="348"/>
+      <c r="G29" s="348"/>
+      <c r="H29" s="348"/>
+      <c r="I29" s="348"/>
+      <c r="J29" s="348"/>
+      <c r="K29" s="348"/>
       <c r="L29" s="17"/>
     </row>
     <row r="30" spans="1:12" ht="12.75" x14ac:dyDescent="0.25">
@@ -12720,12 +12671,12 @@
       <c r="C30" s="39"/>
       <c r="D30" s="42"/>
       <c r="E30" s="38"/>
-      <c r="F30" s="355"/>
-      <c r="G30" s="355"/>
-      <c r="H30" s="355"/>
-      <c r="I30" s="355"/>
-      <c r="J30" s="355"/>
-      <c r="K30" s="355"/>
+      <c r="F30" s="348"/>
+      <c r="G30" s="348"/>
+      <c r="H30" s="348"/>
+      <c r="I30" s="348"/>
+      <c r="J30" s="348"/>
+      <c r="K30" s="348"/>
       <c r="L30" s="17"/>
     </row>
     <row r="31" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -12734,12 +12685,12 @@
       <c r="C31" s="39"/>
       <c r="D31" s="42"/>
       <c r="E31" s="38"/>
-      <c r="F31" s="355"/>
-      <c r="G31" s="355"/>
-      <c r="H31" s="355"/>
-      <c r="I31" s="355"/>
-      <c r="J31" s="355"/>
-      <c r="K31" s="355"/>
+      <c r="F31" s="348"/>
+      <c r="G31" s="348"/>
+      <c r="H31" s="348"/>
+      <c r="I31" s="348"/>
+      <c r="J31" s="348"/>
+      <c r="K31" s="348"/>
       <c r="L31" s="17"/>
     </row>
     <row r="32" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -12959,14 +12910,14 @@
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="78"/>
-      <c r="E2" s="369" t="s">
+      <c r="E2" s="362" t="s">
         <v>67</v>
       </c>
-      <c r="F2" s="369"/>
-      <c r="G2" s="369"/>
-      <c r="H2" s="369"/>
-      <c r="I2" s="369"/>
-      <c r="J2" s="369"/>
+      <c r="F2" s="362"/>
+      <c r="G2" s="362"/>
+      <c r="H2" s="362"/>
+      <c r="I2" s="362"/>
+      <c r="J2" s="362"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="79"/>
@@ -13387,11 +13338,11 @@
       <c r="B28" s="78"/>
       <c r="C28" s="78"/>
       <c r="D28" s="78"/>
-      <c r="E28" s="370" t="s">
+      <c r="E28" s="363" t="s">
         <v>107</v>
       </c>
-      <c r="F28" s="371"/>
-      <c r="G28" s="372"/>
+      <c r="F28" s="364"/>
+      <c r="G28" s="365"/>
       <c r="H28" s="78"/>
       <c r="I28" s="78"/>
       <c r="J28" s="78"/>

</xml_diff>